<commit_message>
Corrige resultados experimentos AQ
</commit_message>
<xml_diff>
--- a/experimentos/resultados.xlsx
+++ b/experimentos/resultados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="AQ_results" sheetId="1" state="visible" r:id="rId2"/>
@@ -244,6 +244,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -265,6 +266,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -345,17 +347,17 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="2" style="0" width="13.6173469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="19.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.4948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="2" style="0" width="13.8214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6632653061225"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="19.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,7 +412,7 @@
         <v>0.0288080404484257</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.0288080404484257</v>
+        <v>-0.0446439316594496</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>0.0288080404484257</v>
@@ -431,7 +433,7 @@
       </c>
       <c r="K2" s="2" t="n">
         <f aca="false">D2</f>
-        <v>0.0288080404484257</v>
+        <v>-0.0446439316594496</v>
       </c>
       <c r="L2" s="2" t="n">
         <f aca="false">E2</f>
@@ -451,46 +453,46 @@
         <v>14</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0653121381610126</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>-0.00477139174436236</v>
+        <v>-0.0700835299053749</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-0.00477139174436236</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-0.00477139174436236</v>
+        <v>-0.0700835299053749</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>-0.083218970414062</v>
+        <v>-0.148531108575075</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0.041408704056413</v>
+        <v>-0.0239034341045996</v>
       </c>
       <c r="I3" s="2" t="n">
         <f aca="false">I2+B3</f>
-        <v>0.020668206501563</v>
+        <v>-0.0446439316594496</v>
       </c>
       <c r="J3" s="2" t="n">
         <f aca="false">J2+C3</f>
-        <v>0.0240366487040633</v>
+        <v>-0.0412754894569493</v>
       </c>
       <c r="K3" s="2" t="n">
         <f aca="false">K2+D3</f>
-        <v>0.0240366487040633</v>
+        <v>-0.0446439316594496</v>
       </c>
       <c r="L3" s="2" t="n">
         <f aca="false">L2+E3</f>
-        <v>0.0240366487040633</v>
+        <v>-0.0412754894569493</v>
       </c>
       <c r="M3" s="2" t="n">
         <f aca="false">M2+F3</f>
-        <v>-0.0680642613208118</v>
+        <v>-0.133376399481824</v>
       </c>
       <c r="N3" s="2" t="n">
         <f aca="false">N2+G3</f>
-        <v>0.053464632711001</v>
+        <v>-0.0118475054500116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,7 +506,7 @@
         <v>0.0720219334998004</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.0607857196363503</v>
+        <v>-0.0087643617075373</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>0.0607857196363503</v>
@@ -518,27 +520,27 @@
       <c r="H4" s="3"/>
       <c r="I4" s="2" t="n">
         <f aca="false">I3+B4</f>
-        <v>0.0119038447940257</v>
+        <v>-0.0534082933669869</v>
       </c>
       <c r="J4" s="2" t="n">
         <f aca="false">J3+C4</f>
-        <v>0.0960585822038637</v>
+        <v>0.0307464440428511</v>
       </c>
       <c r="K4" s="2" t="n">
         <f aca="false">K3+D4</f>
-        <v>0.0848223683404136</v>
+        <v>-0.0534082933669869</v>
       </c>
       <c r="L4" s="2" t="n">
         <f aca="false">L3+E4</f>
-        <v>0.0848223683404136</v>
+        <v>0.0195102301794011</v>
       </c>
       <c r="M4" s="2" t="n">
         <f aca="false">M3+F4</f>
-        <v>-0.093631287057074</v>
+        <v>-0.158943425218087</v>
       </c>
       <c r="N4" s="2" t="n">
         <f aca="false">N3+G4</f>
-        <v>0.0997093142125141</v>
+        <v>0.0343971760515016</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,7 +554,7 @@
         <v>0.105217665970537</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>-0.00203665203952491</v>
+        <v>0.108013138900988</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>-0.00203665203952491</v>
@@ -565,27 +567,27 @@
       </c>
       <c r="I5" s="2" t="n">
         <f aca="false">I4+B5</f>
-        <v>0.132524391439876</v>
+        <v>0.0672122532788633</v>
       </c>
       <c r="J5" s="2" t="n">
         <f aca="false">J4+C5</f>
-        <v>0.201276248174401</v>
+        <v>0.135964110013389</v>
       </c>
       <c r="K5" s="2" t="n">
         <f aca="false">K4+D5</f>
-        <v>0.0827857163008887</v>
+        <v>0.0546048455340008</v>
       </c>
       <c r="L5" s="2" t="n">
         <f aca="false">L4+E5</f>
-        <v>0.0827857163008887</v>
+        <v>0.0174735781398762</v>
       </c>
       <c r="M5" s="2" t="n">
         <f aca="false">M4+F5</f>
-        <v>-0.0153319344541487</v>
+        <v>-0.0806440726151613</v>
       </c>
       <c r="N5" s="2" t="n">
         <f aca="false">N4+G5</f>
-        <v>0.108486607181252</v>
+        <v>0.0431744690202393</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,7 +601,7 @@
         <v>0.29054158741485</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.2620481196488</v>
+        <v>0.193677566673</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>0.2620481196488</v>
@@ -612,27 +614,27 @@
       </c>
       <c r="I6" s="2" t="n">
         <f aca="false">I5+B6</f>
-        <v>0.410372192338776</v>
+        <v>0.345060054177764</v>
       </c>
       <c r="J6" s="2" t="n">
         <f aca="false">J5+C6</f>
-        <v>0.491817835589251</v>
+        <v>0.426505697428238</v>
       </c>
       <c r="K6" s="2" t="n">
         <f aca="false">K5+D6</f>
-        <v>0.344833835949689</v>
+        <v>0.248282412207001</v>
       </c>
       <c r="L6" s="2" t="n">
         <f aca="false">L5+E6</f>
-        <v>0.344833835949689</v>
+        <v>0.279521697788676</v>
       </c>
       <c r="M6" s="2" t="n">
         <f aca="false">M5+F6</f>
-        <v>0.00918572272107644</v>
+        <v>-0.0561264154399361</v>
       </c>
       <c r="N6" s="2" t="n">
         <f aca="false">N5+G6</f>
-        <v>0.0465358756832772</v>
+        <v>-0.0187762624777353</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,7 +648,7 @@
         <v>-0.010859237249924</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.0481850084131884</v>
+        <v>-0.150555304547262</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>0.0481850084131884</v>
@@ -659,27 +661,27 @@
       </c>
       <c r="I7" s="2" t="n">
         <f aca="false">I6+B7</f>
-        <v>0.283339401884014</v>
+        <v>0.218027263723001</v>
       </c>
       <c r="J7" s="2" t="n">
         <f aca="false">J6+C7</f>
-        <v>0.480958598339327</v>
+        <v>0.415646460178314</v>
       </c>
       <c r="K7" s="2" t="n">
         <f aca="false">K6+D7</f>
-        <v>0.393018844362877</v>
+        <v>0.0977271076597388</v>
       </c>
       <c r="L7" s="2" t="n">
         <f aca="false">L6+E7</f>
-        <v>0.393018844362877</v>
+        <v>0.327706706201865</v>
       </c>
       <c r="M7" s="2" t="n">
         <f aca="false">M6+F7</f>
-        <v>-0.0774724547027481</v>
+        <v>-0.142784592863761</v>
       </c>
       <c r="N7" s="2" t="n">
         <f aca="false">N6+G7</f>
-        <v>-0.0477054028124598</v>
+        <v>-0.113017540973472</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,7 +695,7 @@
         <v>-0.167328162431212</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>-0.167328162431212</v>
+        <v>-0.163737569060625</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>-0.167328162431212</v>
@@ -706,27 +708,27 @@
       </c>
       <c r="I8" s="2" t="n">
         <f aca="false">I7+B8</f>
-        <v>0.128558341022652</v>
+        <v>0.0632462028616397</v>
       </c>
       <c r="J8" s="2" t="n">
         <f aca="false">J7+C8</f>
-        <v>0.313630435908115</v>
+        <v>0.248318297747102</v>
       </c>
       <c r="K8" s="2" t="n">
         <f aca="false">K7+D8</f>
-        <v>0.225690681931665</v>
+        <v>-0.0660104614008858</v>
       </c>
       <c r="L8" s="2" t="n">
         <f aca="false">L7+E8</f>
-        <v>0.225690681931665</v>
+        <v>0.160378543770653</v>
       </c>
       <c r="M8" s="2" t="n">
         <f aca="false">M7+F8</f>
-        <v>-0.262458721013835</v>
+        <v>-0.327770859174848</v>
       </c>
       <c r="N8" s="2" t="n">
         <f aca="false">N7+G8</f>
-        <v>-0.21591144481466</v>
+        <v>-0.281223582975672</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,7 +742,7 @@
         <v>-0.00116369479421244</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>-0.00209663657231254</v>
+        <v>0.0124432309833</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>-0.00209663657231254</v>
@@ -753,27 +755,27 @@
       </c>
       <c r="I9" s="2" t="n">
         <f aca="false">I8+B9</f>
-        <v>0.11861332044344</v>
+        <v>0.053301182282427</v>
       </c>
       <c r="J9" s="2" t="n">
         <f aca="false">J8+C9</f>
-        <v>0.312466741113903</v>
+        <v>0.24715460295289</v>
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">K8+D9</f>
-        <v>0.223594045359353</v>
+        <v>-0.0535672304175859</v>
       </c>
       <c r="L9" s="2" t="n">
         <f aca="false">L8+E9</f>
-        <v>0.223594045359353</v>
+        <v>0.15828190719834</v>
       </c>
       <c r="M9" s="2" t="n">
         <f aca="false">M8+F9</f>
-        <v>-0.260691792333023</v>
+        <v>-0.326003930494035</v>
       </c>
       <c r="N9" s="2" t="n">
         <f aca="false">N8+G9</f>
-        <v>-0.212965729287372</v>
+        <v>-0.278277867448385</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,27 +802,27 @@
       </c>
       <c r="I10" s="2" t="n">
         <f aca="false">I9+B10</f>
-        <v>0.11861332044344</v>
+        <v>0.053301182282427</v>
       </c>
       <c r="J10" s="2" t="n">
         <f aca="false">J9+C10</f>
-        <v>0.312466741113903</v>
+        <v>0.24715460295289</v>
       </c>
       <c r="K10" s="2" t="n">
         <f aca="false">K9+D10</f>
-        <v>0.223594045359353</v>
+        <v>-0.0535672304175859</v>
       </c>
       <c r="L10" s="2" t="n">
         <f aca="false">L9+E10</f>
-        <v>0.223594045359353</v>
+        <v>0.15828190719834</v>
       </c>
       <c r="M10" s="2" t="n">
         <f aca="false">M9+F10</f>
-        <v>-0.308290322656597</v>
+        <v>-0.37360246081761</v>
       </c>
       <c r="N10" s="2" t="n">
         <f aca="false">N9+G10</f>
-        <v>-0.212965729287372</v>
+        <v>-0.278277867448385</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -834,7 +836,7 @@
         <v>-0.0514072100259997</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>-0.0722693726074247</v>
+        <v>-0.0454686432291996</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>-0.0722693726074247</v>
@@ -847,27 +849,27 @@
       </c>
       <c r="I11" s="2" t="n">
         <f aca="false">I10+B11</f>
-        <v>0.07314467721424</v>
+        <v>0.00783253905322742</v>
       </c>
       <c r="J11" s="2" t="n">
         <f aca="false">J10+C11</f>
-        <v>0.261059531087903</v>
+        <v>0.19574739292689</v>
       </c>
       <c r="K11" s="2" t="n">
         <f aca="false">K10+D11</f>
-        <v>0.151324672751928</v>
+        <v>-0.0990358736467854</v>
       </c>
       <c r="L11" s="2" t="n">
         <f aca="false">L10+E11</f>
-        <v>0.151324672751928</v>
+        <v>0.0860125345909156</v>
       </c>
       <c r="M11" s="2" t="n">
         <f aca="false">M10+F11</f>
-        <v>-0.356522917460809</v>
+        <v>-0.421835055621822</v>
       </c>
       <c r="N11" s="2" t="n">
         <f aca="false">N10+G11</f>
-        <v>-0.262319694276384</v>
+        <v>-0.327631832437397</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -881,7 +883,7 @@
         <v>0.0115774129006252</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0.0154899118289003</v>
+        <v>0</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>0.0154899118289003</v>
@@ -894,27 +896,27 @@
       </c>
       <c r="I12" s="2" t="n">
         <f aca="false">I11+B12</f>
-        <v>0.07314467721424</v>
+        <v>0.00783253905322742</v>
       </c>
       <c r="J12" s="2" t="n">
         <f aca="false">J11+C12</f>
-        <v>0.272636943988528</v>
+        <v>0.207324805827515</v>
       </c>
       <c r="K12" s="2" t="n">
         <f aca="false">K11+D12</f>
-        <v>0.166814584580828</v>
+        <v>-0.0990358736467854</v>
       </c>
       <c r="L12" s="2" t="n">
         <f aca="false">L11+E12</f>
-        <v>0.166814584580828</v>
+        <v>0.101502446419816</v>
       </c>
       <c r="M12" s="2" t="n">
         <f aca="false">M11+F12</f>
-        <v>-0.342272633175959</v>
+        <v>-0.407584771336972</v>
       </c>
       <c r="N12" s="2" t="n">
         <f aca="false">N11+G12</f>
-        <v>-0.262319694276384</v>
+        <v>-0.327631832437397</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,46 +924,46 @@
         <v>24</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>-0.00855324786157496</v>
+        <v>-0.039822718860175</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0.0427705859324753</v>
+        <v>0.0115011149338753</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0.0312694709986</v>
+        <v>-0.039822718860175</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0.0312694709986</v>
+        <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>-0.0120440227564496</v>
+        <v>-0.0433134937550496</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>-0.0225941904747497</v>
+        <v>-0.0538636614733498</v>
       </c>
       <c r="I13" s="2" t="n">
         <f aca="false">I12+B13</f>
-        <v>0.064591429352665</v>
+        <v>-0.0319901798069476</v>
       </c>
       <c r="J13" s="2" t="n">
         <f aca="false">J12+C13</f>
-        <v>0.315407529921003</v>
+        <v>0.218825920761391</v>
       </c>
       <c r="K13" s="2" t="n">
         <f aca="false">K12+D13</f>
-        <v>0.198084055579428</v>
+        <v>-0.13885859250696</v>
       </c>
       <c r="L13" s="2" t="n">
         <f aca="false">L12+E13</f>
-        <v>0.198084055579428</v>
+        <v>0.101502446419816</v>
       </c>
       <c r="M13" s="2" t="n">
         <f aca="false">M12+F13</f>
-        <v>-0.354316655932409</v>
+        <v>-0.450898265092021</v>
       </c>
       <c r="N13" s="2" t="n">
         <f aca="false">N12+G13</f>
-        <v>-0.284913884751134</v>
+        <v>-0.381495493910747</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,7 +977,7 @@
         <v>0.01278257088345</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0.0197155567207748</v>
+        <v>-0.00188475789767455</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>0.0197155567207748</v>
@@ -988,27 +990,27 @@
       </c>
       <c r="I14" s="2" t="n">
         <f aca="false">I13+B14</f>
-        <v>0.0570286403953154</v>
+        <v>-0.0395529687642972</v>
       </c>
       <c r="J14" s="2" t="n">
         <f aca="false">J13+C14</f>
-        <v>0.328190100804453</v>
+        <v>0.231608491644841</v>
       </c>
       <c r="K14" s="2" t="n">
         <f aca="false">K13+D14</f>
-        <v>0.217799612300203</v>
+        <v>-0.140743350404635</v>
       </c>
       <c r="L14" s="2" t="n">
         <f aca="false">L13+E14</f>
-        <v>0.217799612300203</v>
+        <v>0.121218003140591</v>
       </c>
       <c r="M14" s="2" t="n">
         <f aca="false">M13+F14</f>
-        <v>-0.333376172744309</v>
+        <v>-0.429957781903921</v>
       </c>
       <c r="N14" s="2" t="n">
         <f aca="false">N13+G14</f>
-        <v>-0.248661474880409</v>
+        <v>-0.345243084040022</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,7 +1024,7 @@
         <v>0.0195638262720499</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0.01566353428985</v>
+        <v>0.0134233426732749</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>0.01566353428985</v>
@@ -1035,27 +1037,27 @@
       </c>
       <c r="I15" s="2" t="n">
         <f aca="false">I14+B15</f>
-        <v>0.0704519830685902</v>
+        <v>-0.0261296260910224</v>
       </c>
       <c r="J15" s="2" t="n">
         <f aca="false">J14+C15</f>
-        <v>0.347753927076503</v>
+        <v>0.251172317916891</v>
       </c>
       <c r="K15" s="2" t="n">
         <f aca="false">K14+D15</f>
-        <v>0.233463146590053</v>
+        <v>-0.12732000773136</v>
       </c>
       <c r="L15" s="2" t="n">
         <f aca="false">L14+E15</f>
-        <v>0.233463146590053</v>
+        <v>0.136881537430441</v>
       </c>
       <c r="M15" s="2" t="n">
         <f aca="false">M14+F15</f>
-        <v>-0.302364285820259</v>
+        <v>-0.398945894979871</v>
       </c>
       <c r="N15" s="2" t="n">
         <f aca="false">N14+G15</f>
-        <v>-0.207597555930109</v>
+        <v>-0.304179165089721</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,7 +1071,7 @@
         <v>-0.0424815023587999</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>-0.0497409562600002</v>
+        <v>-0.0095806796875246</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>-0.0497409562600002</v>
@@ -1082,27 +1084,27 @@
       </c>
       <c r="I16" s="2" t="n">
         <f aca="false">I15+B16</f>
-        <v>0.0532712405906156</v>
+        <v>-0.043310368568997</v>
       </c>
       <c r="J16" s="2" t="n">
         <f aca="false">J15+C16</f>
-        <v>0.305272424717703</v>
+        <v>0.208690815558091</v>
       </c>
       <c r="K16" s="2" t="n">
         <f aca="false">K15+D16</f>
-        <v>0.183722190330053</v>
+        <v>-0.136900687418885</v>
       </c>
       <c r="L16" s="2" t="n">
         <f aca="false">L15+E16</f>
-        <v>0.183722190330053</v>
+        <v>0.0871405811704405</v>
       </c>
       <c r="M16" s="2" t="n">
         <f aca="false">M15+F16</f>
-        <v>-0.321252749872784</v>
+        <v>-0.417834359032396</v>
       </c>
       <c r="N16" s="2" t="n">
         <f aca="false">N15+G16</f>
-        <v>-0.217626673317983</v>
+        <v>-0.314208282477596</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,7 +1118,7 @@
         <v>0.0121878371093501</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0.0067676354567</v>
+        <v>0.00792748446512503</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0.0067676354567</v>
@@ -1129,27 +1131,27 @@
       </c>
       <c r="I17" s="2" t="n">
         <f aca="false">I16+B17</f>
-        <v>0.0638754822823156</v>
+        <v>-0.032706126877297</v>
       </c>
       <c r="J17" s="2" t="n">
         <f aca="false">J16+C17</f>
-        <v>0.317460261827053</v>
+        <v>0.220878652667441</v>
       </c>
       <c r="K17" s="2" t="n">
         <f aca="false">K16+D17</f>
-        <v>0.190489825786753</v>
+        <v>-0.12897320295376</v>
       </c>
       <c r="L17" s="2" t="n">
         <f aca="false">L16+E17</f>
-        <v>0.190489825786753</v>
+        <v>0.0939082166271405</v>
       </c>
       <c r="M17" s="2" t="n">
         <f aca="false">M16+F17</f>
-        <v>-0.312024209618483</v>
+        <v>-0.408605818778096</v>
       </c>
       <c r="N17" s="2" t="n">
         <f aca="false">N16+G17</f>
-        <v>-0.223775056716483</v>
+        <v>-0.320356665876096</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1163,7 +1165,7 @@
         <v>-4.16333634234434E-017</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>-4.16333634234434E-017</v>
+        <v>0.022819650385625</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>-4.16333634234434E-017</v>
@@ -1176,27 +1178,27 @@
       </c>
       <c r="I18" s="2" t="n">
         <f aca="false">I17+B18</f>
-        <v>0.0866951326679406</v>
+        <v>-0.00988647649167202</v>
       </c>
       <c r="J18" s="2" t="n">
         <f aca="false">J17+C18</f>
-        <v>0.317460261827053</v>
+        <v>0.220878652667441</v>
       </c>
       <c r="K18" s="2" t="n">
         <f aca="false">K17+D18</f>
-        <v>0.190489825786753</v>
+        <v>-0.106153552568135</v>
       </c>
       <c r="L18" s="2" t="n">
         <f aca="false">L17+E18</f>
-        <v>0.190489825786753</v>
+        <v>0.0939082166271404</v>
       </c>
       <c r="M18" s="2" t="n">
         <f aca="false">M17+F18</f>
-        <v>-0.303642683055983</v>
+        <v>-0.400224292215596</v>
       </c>
       <c r="N18" s="2" t="n">
         <f aca="false">N17+G18</f>
-        <v>-0.223775056716483</v>
+        <v>-0.320356665876096</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,7 +1212,7 @@
         <v>0.00356215517825005</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0.0129832699118748</v>
+        <v>0.00618741288557496</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>0.0129832699118748</v>
@@ -1223,27 +1225,27 @@
       </c>
       <c r="I19" s="2" t="n">
         <f aca="false">I18+B19</f>
-        <v>0.0928825455535156</v>
+        <v>-0.00369906360609706</v>
       </c>
       <c r="J19" s="2" t="n">
         <f aca="false">J18+C19</f>
-        <v>0.321022417005303</v>
+        <v>0.224440807845691</v>
       </c>
       <c r="K19" s="2" t="n">
         <f aca="false">K18+D19</f>
-        <v>0.203473095698628</v>
+        <v>-0.0999661396825597</v>
       </c>
       <c r="L19" s="2" t="n">
         <f aca="false">L18+E19</f>
-        <v>0.203473095698628</v>
+        <v>0.106891486539015</v>
       </c>
       <c r="M19" s="2" t="n">
         <f aca="false">M18+F19</f>
-        <v>-0.266325055321683</v>
+        <v>-0.362906664481296</v>
       </c>
       <c r="N19" s="2" t="n">
         <f aca="false">N18+G19</f>
-        <v>-0.198586476538233</v>
+        <v>-0.295168085697846</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1251,46 +1253,46 @@
         <v>31</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>0.000602875375600088</v>
+        <v>-0.0578137289112999</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.08758535390125</v>
+        <v>0.02916874961435</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>0.08758535390125</v>
+        <v>-0.0578137289112999</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0.08758535390125</v>
+        <v>0.02916874961435</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>0.021513018654775</v>
+        <v>-0.0369035856321249</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>0.0994936863230752</v>
+        <v>0.0410770820361752</v>
       </c>
       <c r="I20" s="2" t="n">
         <f aca="false">I19+B20</f>
-        <v>0.0934854209291156</v>
+        <v>-0.0615127925173969</v>
       </c>
       <c r="J20" s="2" t="n">
         <f aca="false">J19+C20</f>
-        <v>0.408607770906554</v>
+        <v>0.253609557460041</v>
       </c>
       <c r="K20" s="2" t="n">
         <f aca="false">K19+D20</f>
-        <v>0.291058449599878</v>
+        <v>-0.15777986859386</v>
       </c>
       <c r="L20" s="2" t="n">
         <f aca="false">L19+E20</f>
-        <v>0.291058449599878</v>
+        <v>0.136060236153365</v>
       </c>
       <c r="M20" s="2" t="n">
         <f aca="false">M19+F20</f>
-        <v>-0.244812036666908</v>
+        <v>-0.399810250113421</v>
       </c>
       <c r="N20" s="2" t="n">
         <f aca="false">N19+G20</f>
-        <v>-0.0990927902151578</v>
+        <v>-0.25409100366167</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1304,7 +1306,7 @@
         <v>-0.0132910068359245</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>-0.0118313780398745</v>
+        <v>-0.0354782550030247</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>-0.0118313780398745</v>
@@ -1317,27 +1319,27 @@
       </c>
       <c r="I21" s="2" t="n">
         <f aca="false">I20+B21</f>
-        <v>0.0580071659260909</v>
+        <v>-0.0969910475204216</v>
       </c>
       <c r="J21" s="2" t="n">
         <f aca="false">J20+C21</f>
-        <v>0.395316764070629</v>
+        <v>0.240318550624116</v>
       </c>
       <c r="K21" s="2" t="n">
         <f aca="false">K20+D21</f>
-        <v>0.279227071560003</v>
+        <v>-0.193258123596884</v>
       </c>
       <c r="L21" s="2" t="n">
         <f aca="false">L20+E21</f>
-        <v>0.279227071560003</v>
+        <v>0.124228858113491</v>
       </c>
       <c r="M21" s="2" t="n">
         <f aca="false">M20+F21</f>
-        <v>-0.261707094694758</v>
+        <v>-0.416705308141271</v>
       </c>
       <c r="N21" s="2" t="n">
         <f aca="false">N20+G21</f>
-        <v>-0.123533130464508</v>
+        <v>-0.27853134391102</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,46 +1347,46 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>0.0584239118189</v>
+        <v>0.0271867755909252</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0.0493558361277999</v>
+        <v>0.0181186998998251</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0.0572751740284501</v>
+        <v>0.0354936559695254</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>0.0572751740284501</v>
+        <v>0.0260380378004752</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0.0460944750000001</v>
+        <v>0.0148573387720252</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>0.046950961227975</v>
+        <v>0.0157138250000002</v>
       </c>
       <c r="I22" s="2" t="n">
         <f aca="false">I21+B22</f>
-        <v>0.116431077744991</v>
+        <v>-0.0698042719294965</v>
       </c>
       <c r="J22" s="2" t="n">
         <f aca="false">J21+C22</f>
-        <v>0.444672600198429</v>
+        <v>0.258437250523941</v>
       </c>
       <c r="K22" s="2" t="n">
         <f aca="false">K21+D22</f>
-        <v>0.336502245588453</v>
+        <v>-0.157764467627359</v>
       </c>
       <c r="L22" s="2" t="n">
         <f aca="false">L21+E22</f>
-        <v>0.336502245588453</v>
+        <v>0.150266895913966</v>
       </c>
       <c r="M22" s="2" t="n">
         <f aca="false">M21+F22</f>
-        <v>-0.215612619694758</v>
+        <v>-0.401847969369246</v>
       </c>
       <c r="N22" s="2" t="n">
         <f aca="false">N21+G22</f>
-        <v>-0.0765821692365327</v>
+        <v>-0.26281751891102</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,7 +1400,7 @@
         <v>-0.0052611227464246</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>0.00331073105967511</v>
+        <v>-0.00357938964344956</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>0.00331073105967511</v>
@@ -1411,27 +1413,27 @@
       </c>
       <c r="I23" s="2" t="n">
         <f aca="false">I22+B23</f>
-        <v>0.113041213101541</v>
+        <v>-0.0731941365729461</v>
       </c>
       <c r="J23" s="2" t="n">
         <f aca="false">J22+C23</f>
-        <v>0.439411477452004</v>
+        <v>0.253176127777517</v>
       </c>
       <c r="K23" s="2" t="n">
         <f aca="false">K22+D23</f>
-        <v>0.339812976648128</v>
+        <v>-0.161343857270808</v>
       </c>
       <c r="L23" s="2" t="n">
         <f aca="false">L22+E23</f>
-        <v>0.339812976648128</v>
+        <v>0.153577626973641</v>
       </c>
       <c r="M23" s="2" t="n">
         <f aca="false">M22+F23</f>
-        <v>-0.228108395476033</v>
+        <v>-0.41434374515052</v>
       </c>
       <c r="N23" s="2" t="n">
         <f aca="false">N22+G23</f>
-        <v>-0.0921855761726576</v>
+        <v>-0.278420925847145</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,46 +1441,46 @@
         <v>35</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>0.0475593719751749</v>
+        <v>0</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.0475593719751749</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>0.0475593719751749</v>
+        <v>0</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0.0475593719751749</v>
+        <v>0</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>0.0475593719751749</v>
+        <v>0</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>0.0475593719751749</v>
+        <v>0</v>
       </c>
       <c r="I24" s="2" t="n">
         <f aca="false">I23+B24</f>
-        <v>0.160600585076716</v>
+        <v>-0.0731941365729461</v>
       </c>
       <c r="J24" s="2" t="n">
         <f aca="false">J23+C24</f>
-        <v>0.486970849427179</v>
+        <v>0.253176127777517</v>
       </c>
       <c r="K24" s="2" t="n">
         <f aca="false">K23+D24</f>
-        <v>0.387372348623303</v>
+        <v>-0.161343857270808</v>
       </c>
       <c r="L24" s="2" t="n">
         <f aca="false">L23+E24</f>
-        <v>0.387372348623303</v>
+        <v>0.153577626973641</v>
       </c>
       <c r="M24" s="2" t="n">
         <f aca="false">M23+F24</f>
-        <v>-0.180549023500858</v>
+        <v>-0.41434374515052</v>
       </c>
       <c r="N24" s="2" t="n">
         <f aca="false">N23+G24</f>
-        <v>-0.0446262041974827</v>
+        <v>-0.278420925847145</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,46 +1488,46 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0.0892800730368751</v>
+        <v>0.0342201545823253</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.07742224833735</v>
+        <v>0.0223623298828002</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>-0.0184853794922</v>
+        <v>-0.0624635318309745</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>-0.0184853794922</v>
+        <v>-0.0735452979467498</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>0.0767802828125249</v>
+        <v>0.0217203643579751</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>0.0683403225561</v>
+        <v>0.0132804041015502</v>
       </c>
       <c r="I25" s="2" t="n">
         <f aca="false">I24+B25</f>
-        <v>0.249880658113591</v>
+        <v>-0.0389739819906208</v>
       </c>
       <c r="J25" s="2" t="n">
         <f aca="false">J24+C25</f>
-        <v>0.564393097764529</v>
+        <v>0.275538457660317</v>
       </c>
       <c r="K25" s="2" t="n">
         <f aca="false">K24+D25</f>
-        <v>0.368886969131103</v>
+        <v>-0.223807389101783</v>
       </c>
       <c r="L25" s="2" t="n">
         <f aca="false">L24+E25</f>
-        <v>0.368886969131103</v>
+        <v>0.0800323290268912</v>
       </c>
       <c r="M25" s="2" t="n">
         <f aca="false">M24+F25</f>
-        <v>-0.103768740688333</v>
+        <v>-0.392623380792545</v>
       </c>
       <c r="N25" s="2" t="n">
         <f aca="false">N24+G25</f>
-        <v>0.0237141183586172</v>
+        <v>-0.265140521745595</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1539,7 +1541,7 @@
         <v>-0.0127866752955247</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>-0.0136905821514249</v>
+        <v>-0.0265632264823748</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>-0.0136905821514249</v>
@@ -1552,27 +1554,27 @@
       </c>
       <c r="I26" s="2" t="n">
         <f aca="false">I25+B26</f>
-        <v>0.233197585642641</v>
+        <v>-0.0556570544615708</v>
       </c>
       <c r="J26" s="2" t="n">
         <f aca="false">J25+C26</f>
-        <v>0.551606422469004</v>
+        <v>0.262751782364792</v>
       </c>
       <c r="K26" s="2" t="n">
         <f aca="false">K25+D26</f>
-        <v>0.355196386979678</v>
+        <v>-0.250370615584158</v>
       </c>
       <c r="L26" s="2" t="n">
         <f aca="false">L25+E26</f>
-        <v>0.355196386979678</v>
+        <v>0.0663417468754663</v>
       </c>
       <c r="M26" s="2" t="n">
         <f aca="false">M25+F26</f>
-        <v>-0.111677935885732</v>
+        <v>-0.400532575989945</v>
       </c>
       <c r="N26" s="2" t="n">
         <f aca="false">N25+G26</f>
-        <v>-0.00304277099938277</v>
+        <v>-0.291897411103595</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,7 +1588,7 @@
         <v>0.00230479355965022</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>0.00748396161857504</v>
+        <v>-0.00433576854472503</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>0.00748396161857504</v>
@@ -1599,27 +1601,27 @@
       </c>
       <c r="I27" s="2" t="n">
         <f aca="false">I26+B27</f>
-        <v>0.243321357026791</v>
+        <v>-0.0455332830774207</v>
       </c>
       <c r="J27" s="2" t="n">
         <f aca="false">J26+C27</f>
-        <v>0.553911216028655</v>
+        <v>0.265056575924443</v>
       </c>
       <c r="K27" s="2" t="n">
         <f aca="false">K26+D27</f>
-        <v>0.362680348598253</v>
+        <v>-0.254706384128883</v>
       </c>
       <c r="L27" s="2" t="n">
         <f aca="false">L26+E27</f>
-        <v>0.362680348598253</v>
+        <v>0.0738257084940413</v>
       </c>
       <c r="M27" s="2" t="n">
         <f aca="false">M26+F27</f>
-        <v>-0.114708331093107</v>
+        <v>-0.403562971197319</v>
       </c>
       <c r="N27" s="2" t="n">
         <f aca="false">N26+G27</f>
-        <v>-0.00422958191193253</v>
+        <v>-0.293084222016145</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,27 +1648,27 @@
       </c>
       <c r="I28" s="2" t="n">
         <f aca="false">I27+B28</f>
-        <v>0.243321357026791</v>
+        <v>-0.0455332830774207</v>
       </c>
       <c r="J28" s="2" t="n">
         <f aca="false">J27+C28</f>
-        <v>0.553911216028655</v>
+        <v>0.265056575924443</v>
       </c>
       <c r="K28" s="2" t="n">
         <f aca="false">K27+D28</f>
-        <v>0.362680348598253</v>
+        <v>-0.254706384128883</v>
       </c>
       <c r="L28" s="2" t="n">
         <f aca="false">L27+E28</f>
-        <v>0.362680348598253</v>
+        <v>0.0738257084940413</v>
       </c>
       <c r="M28" s="2" t="n">
         <f aca="false">M27+F28</f>
-        <v>-0.0988505165348322</v>
+        <v>-0.387705156639044</v>
       </c>
       <c r="N28" s="2" t="n">
         <f aca="false">N27+G28</f>
-        <v>-0.00422958191193253</v>
+        <v>-0.293084222016145</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,7 +1682,7 @@
         <v>-0.00431091445312511</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>-0.00431091445312511</v>
+        <v>-0.01291382490985</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>-0.00431091445312511</v>
@@ -1693,27 +1695,27 @@
       </c>
       <c r="I29" s="2" t="n">
         <f aca="false">I28+B29</f>
-        <v>0.230407532116941</v>
+        <v>-0.0584471079872707</v>
       </c>
       <c r="J29" s="2" t="n">
         <f aca="false">J28+C29</f>
-        <v>0.549600301575529</v>
+        <v>0.260745661471317</v>
       </c>
       <c r="K29" s="2" t="n">
         <f aca="false">K28+D29</f>
-        <v>0.358369434145128</v>
+        <v>-0.267620209038733</v>
       </c>
       <c r="L29" s="2" t="n">
         <f aca="false">L28+E29</f>
-        <v>0.358369434145128</v>
+        <v>0.0695147940409162</v>
       </c>
       <c r="M29" s="2" t="n">
         <f aca="false">M28+F29</f>
-        <v>-0.108254985680457</v>
+        <v>-0.397109625784669</v>
       </c>
       <c r="N29" s="2" t="n">
         <f aca="false">N28+G29</f>
-        <v>0.00540998977274272</v>
+        <v>-0.283444650331469</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,7 +1729,7 @@
         <v>0.00732796230967501</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>0.00732796230967501</v>
+        <v>0.00157834892827511</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>0.00732796230967501</v>
@@ -1740,27 +1742,27 @@
       </c>
       <c r="I30" s="2" t="n">
         <f aca="false">I29+B30</f>
-        <v>0.237735494426616</v>
+        <v>-0.0511191456775957</v>
       </c>
       <c r="J30" s="2" t="n">
         <f aca="false">J29+C30</f>
-        <v>0.556928263885204</v>
+        <v>0.268073623780992</v>
       </c>
       <c r="K30" s="2" t="n">
         <f aca="false">K29+D30</f>
-        <v>0.365697396454803</v>
+        <v>-0.266041860110458</v>
       </c>
       <c r="L30" s="2" t="n">
         <f aca="false">L29+E30</f>
-        <v>0.365697396454803</v>
+        <v>0.0768427563505912</v>
       </c>
       <c r="M30" s="2" t="n">
         <f aca="false">M29+F30</f>
-        <v>-0.106676636752182</v>
+        <v>-0.395531276856394</v>
       </c>
       <c r="N30" s="2" t="n">
         <f aca="false">N29+G30</f>
-        <v>0.0255848168160177</v>
+        <v>-0.263269823288194</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,46 +1770,46 @@
         <v>42</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>0.0262467167943873</v>
+        <v>0</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>0.0416463434520624</v>
+        <v>0.015399626657675</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>0.0416353002829874</v>
+        <v>0</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0.0416353002829874</v>
+        <v>0.0153885834886001</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>0.0416353002829874</v>
+        <v>0.0153885834886001</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>0.0262467167943873</v>
+        <v>0</v>
       </c>
       <c r="I31" s="2" t="n">
         <f aca="false">I30+B31</f>
-        <v>0.263982211221004</v>
+        <v>-0.0511191456775957</v>
       </c>
       <c r="J31" s="2" t="n">
         <f aca="false">J30+C31</f>
-        <v>0.598574607337267</v>
+        <v>0.283473250438668</v>
       </c>
       <c r="K31" s="2" t="n">
         <f aca="false">K30+D31</f>
-        <v>0.407332696737791</v>
+        <v>-0.266041860110458</v>
       </c>
       <c r="L31" s="2" t="n">
         <f aca="false">L30+E31</f>
-        <v>0.407332696737791</v>
+        <v>0.0922313398391913</v>
       </c>
       <c r="M31" s="2" t="n">
         <f aca="false">M30+F31</f>
-        <v>-0.0650413364691947</v>
+        <v>-0.380142693367794</v>
       </c>
       <c r="N31" s="2" t="n">
         <f aca="false">N30+G31</f>
-        <v>0.051831533610405</v>
+        <v>-0.263269823288194</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1821,7 +1823,7 @@
         <v>-0.0118542398487502</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>-0.0118542398487502</v>
+        <v>0.00277195898437518</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>-0.0118542398487502</v>
@@ -1834,27 +1836,27 @@
       </c>
       <c r="I32" s="2" t="n">
         <f aca="false">I31+B32</f>
-        <v>0.267583887593179</v>
+        <v>-0.0475174693054205</v>
       </c>
       <c r="J32" s="2" t="n">
         <f aca="false">J31+C32</f>
-        <v>0.586720367488517</v>
+        <v>0.271619010589917</v>
       </c>
       <c r="K32" s="2" t="n">
         <f aca="false">K31+D32</f>
-        <v>0.395478456889041</v>
+        <v>-0.263269901126082</v>
       </c>
       <c r="L32" s="2" t="n">
         <f aca="false">L31+E32</f>
-        <v>0.395478456889041</v>
+        <v>0.0803770999904411</v>
       </c>
       <c r="M32" s="2" t="n">
         <f aca="false">M31+F32</f>
-        <v>-0.0583114104976448</v>
+        <v>-0.373412767396244</v>
       </c>
       <c r="N32" s="2" t="n">
         <f aca="false">N31+G32</f>
-        <v>0.0399772937616549</v>
+        <v>-0.275124063136944</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,7 +1870,7 @@
         <v>-0.00558019228764981</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>-0.00558019228764981</v>
+        <v>0.00842755801782516</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>-0.00558019228764981</v>
@@ -1881,27 +1883,27 @@
       </c>
       <c r="I33" s="2" t="n">
         <f aca="false">I32+B33</f>
-        <v>0.290918165628029</v>
+        <v>-0.0241831912705702</v>
       </c>
       <c r="J33" s="2" t="n">
         <f aca="false">J32+C33</f>
-        <v>0.581140175200867</v>
+        <v>0.266038818302268</v>
       </c>
       <c r="K33" s="2" t="n">
         <f aca="false">K32+D33</f>
-        <v>0.389898264601391</v>
+        <v>-0.254842343108257</v>
       </c>
       <c r="L33" s="2" t="n">
         <f aca="false">L32+E33</f>
-        <v>0.389898264601391</v>
+        <v>0.0747969077027913</v>
       </c>
       <c r="M33" s="2" t="n">
         <f aca="false">M32+F33</f>
-        <v>-0.0216401336446945</v>
+        <v>-0.336741490543294</v>
       </c>
       <c r="N33" s="2" t="n">
         <f aca="false">N32+G33</f>
-        <v>0.0843627966011802</v>
+        <v>-0.230738560297419</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1915,7 +1917,7 @@
         <v>-0.00972682567610002</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>-0.00732962860577487</v>
+        <v>0.00155555341047501</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>-0.00732962860577487</v>
@@ -1928,27 +1930,27 @@
       </c>
       <c r="I34" s="2" t="n">
         <f aca="false">I33+B34</f>
-        <v>0.289018820891479</v>
+        <v>-0.0260825360071202</v>
       </c>
       <c r="J34" s="2" t="n">
         <f aca="false">J33+C34</f>
-        <v>0.571413349524767</v>
+        <v>0.256311992626168</v>
       </c>
       <c r="K34" s="2" t="n">
         <f aca="false">K33+D34</f>
-        <v>0.382568635995616</v>
+        <v>-0.253286789697782</v>
       </c>
       <c r="L34" s="2" t="n">
         <f aca="false">L33+E34</f>
-        <v>0.382568635995616</v>
+        <v>0.0674672790970165</v>
       </c>
       <c r="M34" s="2" t="n">
         <f aca="false">M33+F34</f>
-        <v>-0.0250935653804949</v>
+        <v>-0.340194922279094</v>
       </c>
       <c r="N34" s="2" t="n">
         <f aca="false">N33+G34</f>
-        <v>0.100739703231805</v>
+        <v>-0.214361653666794</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,46 +1958,46 @@
         <v>46</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>-0.020896875876375</v>
+        <v>-0.0913916513671748</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>-0.0246954518579751</v>
+        <v>-0.0951902273487749</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>-0.0246954518579751</v>
+        <v>-0.0923554627904748</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>-0.0246954518579751</v>
+        <v>-0.0951902273487749</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>-0.00837944462142487</v>
+        <v>-0.0788742201122247</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>-0.028341262394825</v>
+        <v>-0.0988360378856248</v>
       </c>
       <c r="I35" s="2" t="n">
         <f aca="false">I34+B35</f>
-        <v>0.268121945015104</v>
+        <v>-0.117474187374295</v>
       </c>
       <c r="J35" s="2" t="n">
         <f aca="false">J34+C35</f>
-        <v>0.546717897666792</v>
+        <v>0.161121765277393</v>
       </c>
       <c r="K35" s="2" t="n">
         <f aca="false">K34+D35</f>
-        <v>0.357873184137641</v>
+        <v>-0.345642252488257</v>
       </c>
       <c r="L35" s="2" t="n">
         <f aca="false">L34+E35</f>
-        <v>0.357873184137641</v>
+        <v>-0.0277229482517585</v>
       </c>
       <c r="M35" s="2" t="n">
         <f aca="false">M34+F35</f>
-        <v>-0.0334730100019197</v>
+        <v>-0.419069142391319</v>
       </c>
       <c r="N35" s="2" t="n">
         <f aca="false">N34+G35</f>
-        <v>0.07239844083698</v>
+        <v>-0.313197691552419</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,7 +2011,7 @@
         <v>-0.0482734785256749</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>-0.0482734785256749</v>
+        <v>-0.0299966226562747</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>-0.0482734785256749</v>
@@ -2022,27 +2024,27 @@
       </c>
       <c r="I36" s="2" t="n">
         <f aca="false">I35+B36</f>
-        <v>0.217917063174154</v>
+        <v>-0.167679069215245</v>
       </c>
       <c r="J36" s="2" t="n">
         <f aca="false">J35+C36</f>
-        <v>0.498444419141117</v>
+        <v>0.112848286751718</v>
       </c>
       <c r="K36" s="2" t="n">
         <f aca="false">K35+D36</f>
-        <v>0.309599705611966</v>
+        <v>-0.375638875144532</v>
       </c>
       <c r="L36" s="2" t="n">
         <f aca="false">L35+E36</f>
-        <v>0.309599705611966</v>
+        <v>-0.0759964267774334</v>
       </c>
       <c r="M36" s="2" t="n">
         <f aca="false">M35+F36</f>
-        <v>-0.0605328365544693</v>
+        <v>-0.446128968943868</v>
       </c>
       <c r="N36" s="2" t="n">
         <f aca="false">N35+G36</f>
-        <v>0.0414181275656803</v>
+        <v>-0.344178004823719</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,27 +2053,27 @@
       </c>
       <c r="B38" s="3" t="n">
         <f aca="false">AVERAGE(B2:B36)</f>
-        <v>0.00622620180497584</v>
+        <v>-0.00479083054900699</v>
       </c>
       <c r="C38" s="3" t="n">
         <f aca="false">AVERAGE(C2:C36)</f>
-        <v>0.0142412691183176</v>
+        <v>0.00322423676433479</v>
       </c>
       <c r="D38" s="3" t="n">
         <f aca="false">AVERAGE(D2:D36)</f>
-        <v>0.0088457058746276</v>
+        <v>-0.0107325392898438</v>
       </c>
       <c r="E38" s="3" t="n">
         <f aca="false">AVERAGE(E2:E36)</f>
-        <v>0.0088457058746276</v>
+        <v>-0.00217132647935524</v>
       </c>
       <c r="F38" s="3" t="n">
         <f aca="false">AVERAGE(F2:F36)</f>
-        <v>-0.00172950961584198</v>
+        <v>-0.0127465419698248</v>
       </c>
       <c r="G38" s="3" t="n">
         <f aca="false">AVERAGE(G2:G36)</f>
-        <v>0.00118337507330515</v>
+        <v>-0.00983365728067768</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,27 +2082,27 @@
       </c>
       <c r="B39" s="3" t="n">
         <f aca="false">STDEV(B2:B36)</f>
-        <v>0.0685974353221723</v>
+        <v>0.0678718634319329</v>
       </c>
       <c r="C39" s="3" t="n">
         <f aca="false">STDEV(C2:C36)</f>
-        <v>0.0671723460255843</v>
+        <v>0.0672153405120472</v>
       </c>
       <c r="D39" s="3" t="n">
         <f aca="false">STDEV(D2:D36)</f>
-        <v>0.0617136080337497</v>
+        <v>0.0597982134138702</v>
       </c>
       <c r="E39" s="3" t="n">
         <f aca="false">STDEV(E2:E36)</f>
-        <v>0.0617136080337497</v>
+        <v>0.0633183408623461</v>
       </c>
       <c r="F39" s="3" t="n">
         <f aca="false">STDEV(F2:F36)</f>
-        <v>0.0484925986672177</v>
+        <v>0.0506432990351528</v>
       </c>
       <c r="G39" s="3" t="n">
         <f aca="false">STDEV(G2:G36)</f>
-        <v>0.0478022850348901</v>
+        <v>0.0443765131719409</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2125,7 +2127,7 @@
       </c>
       <c r="F40" s="3" t="n">
         <f aca="false">MEDIAN(F2:F36)</f>
-        <v>0.0017669286808126</v>
+        <v>0</v>
       </c>
       <c r="G40" s="3" t="n">
         <f aca="false">MEDIAN(G2:G36)</f>
@@ -2146,7 +2148,7 @@
       </c>
       <c r="D41" s="3" t="n">
         <f aca="false">MIN(D2:D36)</f>
-        <v>-0.167328162431212</v>
+        <v>-0.163737569060625</v>
       </c>
       <c r="E41" s="3" t="n">
         <f aca="false">MIN(E2:E36)</f>
@@ -2175,7 +2177,7 @@
       </c>
       <c r="D42" s="3" t="n">
         <f aca="false">MAX(D2:D36)</f>
-        <v>0.2620481196488</v>
+        <v>0.193677566673</v>
       </c>
       <c r="E42" s="3" t="n">
         <f aca="false">MAX(E2:E36)</f>
@@ -2187,7 +2189,7 @@
       </c>
       <c r="G42" s="3" t="n">
         <f aca="false">MAX(G2:G36)</f>
-        <v>0.0994936863230752</v>
+        <v>0.0462446815015131</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2198,7 @@
       </c>
       <c r="B43" s="0" t="n">
         <f aca="false">COUNTIF(B2:B36,"&gt;=0")</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C43" s="0" t="n">
         <f aca="false">COUNTIF(C2:C36,"&gt;=0")</f>
@@ -2204,7 +2206,7 @@
       </c>
       <c r="D43" s="0" t="n">
         <f aca="false">COUNTIF(D2:D36,"&gt;=0")</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E43" s="0" t="n">
         <f aca="false">COUNTIF(E2:E36,"&gt;=0")</f>
@@ -2212,11 +2214,11 @@
       </c>
       <c r="F43" s="0" t="n">
         <f aca="false">COUNTIF(F2:F36,"&gt;=0")</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G43" s="0" t="n">
         <f aca="false">COUNTIF(G2:G36,"&gt;=0")</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,7 +2227,7 @@
       </c>
       <c r="B44" s="0" t="n">
         <f aca="false">COUNTIF(B2:B36,"&lt;0")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C44" s="0" t="n">
         <f aca="false">COUNTIF(C2:C36,"&lt;0")</f>
@@ -2233,7 +2235,7 @@
       </c>
       <c r="D44" s="0" t="n">
         <f aca="false">COUNTIF(D2:D36,"&lt;0")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E44" s="0" t="n">
         <f aca="false">COUNTIF(E2:E36,"&lt;0")</f>
@@ -2241,11 +2243,11 @@
       </c>
       <c r="F44" s="0" t="n">
         <f aca="false">COUNTIF(F2:F36,"&lt;0")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G44" s="0" t="n">
         <f aca="false">COUNTIF(G2:G36,"&lt;0")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2266,17 +2268,17 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.984693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2335,7 +2337,7 @@
       </c>
       <c r="I2" s="3" t="n">
         <f aca="false">HLOOKUP(A2,AQ_results!$A$1:$G$44,38,0)</f>
-        <v>0.00622620180497584</v>
+        <v>-0.00479083054900699</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,7 +2367,7 @@
       </c>
       <c r="I3" s="3" t="n">
         <f aca="false">HLOOKUP(A3,AQ_results!$A$1:$G$44,38,0)</f>
-        <v>0.0142412691183176</v>
+        <v>0.00322423676433479</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2395,7 +2397,7 @@
       </c>
       <c r="I4" s="3" t="n">
         <f aca="false">HLOOKUP(A4,AQ_results!$A$1:$G$44,38,0)</f>
-        <v>0.0088457058746276</v>
+        <v>-0.0107325392898438</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,7 +2427,7 @@
       </c>
       <c r="I5" s="3" t="n">
         <f aca="false">HLOOKUP(A5,AQ_results!$A$1:$G$44,38,0)</f>
-        <v>0.0088457058746276</v>
+        <v>-0.00217132647935524</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2455,7 +2457,7 @@
       </c>
       <c r="I6" s="3" t="n">
         <f aca="false">HLOOKUP(A6,AQ_results!$A$1:$G$44,38,0)</f>
-        <v>-0.00172950961584198</v>
+        <v>-0.0127465419698248</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,13 +2487,13 @@
       </c>
       <c r="I7" s="3" t="n">
         <f aca="false">HLOOKUP(A7,AQ_results!$A$1:$G$44,38,0)</f>
-        <v>0.00118337507330515</v>
+        <v>-0.00983365728067768</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Agrega resultados con AQ para la versión mod de BH
</commit_message>
<xml_diff>
--- a/experimentos/resultados.xlsx
+++ b/experimentos/resultados.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="AQ_results" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="AQ_descrip" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="CN2_results" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="CN2_descrip" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Observaciones" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="88">
   <si>
     <t>File</t>
   </si>
@@ -46,6 +47,192 @@
     <t>Exp_6_Ex_Ret</t>
   </si>
   <si>
+    <t>Exp_1_Ex_Ret_BH_mod</t>
+  </si>
+  <si>
+    <t>Exp_2_Ex_Ret_BH_Mod</t>
+  </si>
+  <si>
+    <t>Exp_3_Ex_Ret_BH_Mod</t>
+  </si>
+  <si>
+    <t>Exp_4_Ex_Ret_BH_Mod</t>
+  </si>
+  <si>
+    <t>Exp_5_Ex_Ret_BH_Mod</t>
+  </si>
+  <si>
+    <t>Exp_6_Ex_Ret_BH_Mod</t>
+  </si>
+  <si>
+    <t>2_ipc_2007-05-16_2007-09-18_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>3_ipc_2007-09-19_2008-01-30_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>4_ipc_2008-01-31_2008-06-11_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>5_ipc_2008-06-12_2008-10-16_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>6_ipc_2008-10-17_2009-02-26_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>7_ipc_2009-02-27_2009-07-08_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>8_ipc_2009-07-09_2009-11-13_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>9_ipc_2009-11-17_2010-03-26_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>10_ipc_2010-03-29_2010-08-04_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>11_ipc_2010-08-05_2010-12-14_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>12_ipc_2010-12-15_2011-04-27_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>13_ipc_2011-04-28_2011-08-31_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>14_ipc_2011-09-01_2012-01-12_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>15_ipc_2012-01-13_2012-05-24_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>16_ipc_2012-05-25_2012-10-01_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>17_ipc_2012-10-02_2013-02-14_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>18_ipc_2013-02-15_2013-06-26_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>19_ipc_2013-06-27_2013-10-31_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>20_ipc_2013-11-01_2014-03-18_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>21_ipc_2014-03-19_2014-07-25_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>22_ipc_2014-07-28_2014-12-02_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>23_ipc_2014-12-03_2015-04-24_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>24_ipc_2015-04-27_2015-08-31_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>25_ipc_2015-09-01_2016-01-11_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>26_ipc_2016-01-12_2016-05-20_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>27_ipc_2016-05-23_2016-09-26_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>28_ipc_2016-09-27_2017-02-02_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>29_ipc_2017-02-03_2017-06-15_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>30_ipc_2017-06-16_2017-10-20_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>31_ipc_2017-10-23_2018-03-05_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>32_ipc_2018-03-06_2018-07-13_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>33_ipc_2018-07-16_2018-11-20_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>34_ipc_2018-11-21_2019-04-02_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>35_ipc_2019-04-03_2019-08-09_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>36_ipc_2019-08-12_2019-12-18_90_predicciones.csv</t>
+  </si>
+  <si>
+    <t>Promedio</t>
+  </si>
+  <si>
+    <t>Desviación estándar</t>
+  </si>
+  <si>
+    <t>Mediana</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Número de casos no negativos</t>
+  </si>
+  <si>
+    <t>Número de casos negativos</t>
+  </si>
+  <si>
+    <t>Experimento</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Precio Ejecución</t>
+  </si>
+  <si>
+    <t>Discretización</t>
+  </si>
+  <si>
+    <t>Lim Inf</t>
+  </si>
+  <si>
+    <t>Lim Sup</t>
+  </si>
+  <si>
+    <t>Penaliza?</t>
+  </si>
+  <si>
+    <t>Acumula?</t>
+  </si>
+  <si>
+    <t>Ex Ret</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>Cuantiles</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Intervalos</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Exp_1_Ex_Ret_Acum</t>
   </si>
   <si>
@@ -64,182 +251,54 @@
     <t>Exp_6_Ex_Ret_Acum</t>
   </si>
   <si>
-    <t>2_ipc_2007-05-16_2007-09-18_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>3_ipc_2007-09-19_2008-01-30_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>4_ipc_2008-01-31_2008-06-11_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>5_ipc_2008-06-12_2008-10-16_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>6_ipc_2008-10-17_2009-02-26_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>7_ipc_2009-02-27_2009-07-08_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>8_ipc_2009-07-09_2009-11-13_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>9_ipc_2009-11-17_2010-03-26_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>10_ipc_2010-03-29_2010-08-04_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>11_ipc_2010-08-05_2010-12-14_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>12_ipc_2010-12-15_2011-04-27_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>13_ipc_2011-04-28_2011-08-31_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>14_ipc_2011-09-01_2012-01-12_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>15_ipc_2012-01-13_2012-05-24_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>16_ipc_2012-05-25_2012-10-01_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>17_ipc_2012-10-02_2013-02-14_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>18_ipc_2013-02-15_2013-06-26_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>19_ipc_2013-06-27_2013-10-31_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>20_ipc_2013-11-01_2014-03-18_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>21_ipc_2014-03-19_2014-07-25_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>22_ipc_2014-07-28_2014-12-02_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>23_ipc_2014-12-03_2015-04-24_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>24_ipc_2015-04-27_2015-08-31_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>25_ipc_2015-09-01_2016-01-11_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>26_ipc_2016-01-12_2016-05-20_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>27_ipc_2016-05-23_2016-09-26_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>28_ipc_2016-09-27_2017-02-02_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>29_ipc_2017-02-03_2017-06-15_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>30_ipc_2017-06-16_2017-10-20_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>31_ipc_2017-10-23_2018-03-05_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>32_ipc_2018-03-06_2018-07-13_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>33_ipc_2018-07-16_2018-11-20_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>34_ipc_2018-11-21_2019-04-02_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>35_ipc_2019-04-03_2019-08-09_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>36_ipc_2019-08-12_2019-12-18_90_predicciones.csv</t>
-  </si>
-  <si>
-    <t>Promedio</t>
-  </si>
-  <si>
-    <t>Desviación estándar</t>
-  </si>
-  <si>
-    <t>Mediana</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Número de casos no negativos</t>
-  </si>
-  <si>
-    <t>Número de casos negativos</t>
-  </si>
-  <si>
-    <t>Experimento</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>Precio Ejecución</t>
-  </si>
-  <si>
-    <t>Discretización</t>
-  </si>
-  <si>
-    <t>Lim Inf</t>
-  </si>
-  <si>
-    <t>Lim Sup</t>
-  </si>
-  <si>
-    <t>Penaliza?</t>
-  </si>
-  <si>
-    <t>Acumula?</t>
-  </si>
-  <si>
-    <t>Ex Ret</t>
-  </si>
-  <si>
-    <t>mid</t>
-  </si>
-  <si>
-    <t>Cuantiles</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>Intervalos</t>
-  </si>
-  <si>
-    <t>No</t>
+    <t>Posición de la bandas en función de BH</t>
+  </si>
+  <si>
+    <t>Lunes y Miércoles</t>
+  </si>
+  <si>
+    <t>Las bandas están en función del costo de operación</t>
+  </si>
+  <si>
+    <t>Viernes después de seminario</t>
+  </si>
+  <si>
+    <t>Criterio para considerar si ya se llevan muchas operaciones (pérdidas)</t>
+  </si>
+  <si>
+    <t>Compra al inicio del periodo (suena a cucharear)</t>
+  </si>
+  <si>
+    <t>prioridad</t>
+  </si>
+  <si>
+    <t>Probar otros límites (límites en función de la varianza del periodo de entrenamiento)</t>
+  </si>
+  <si>
+    <t>Separar mercados a la alza y a la baja</t>
+  </si>
+  <si>
+    <t>Escrito (Introducción y estado del arte)</t>
+  </si>
+  <si>
+    <t>Salvador</t>
+  </si>
+  <si>
+    <t>Pensar lo que implicaría bloques deslizantes</t>
+  </si>
+  <si>
+    <t>Próxima</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00%;[RED]\-0.00%"/>
-    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -313,7 +372,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -327,6 +386,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -349,17 +412,16 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="2" style="0" width="13.9336734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.7704081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="20.1938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="2" style="0" width="14.1479591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="22.4183673469388"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,28 +487,23 @@
       <c r="G2" s="2" t="n">
         <v>0.012055928654588</v>
       </c>
+      <c r="H2" s="3"/>
       <c r="I2" s="2" t="n">
-        <f aca="false">B2</f>
         <v>-0.0446439316594496</v>
       </c>
       <c r="J2" s="2" t="n">
-        <f aca="false">C2</f>
         <v>0.0288080404484257</v>
       </c>
       <c r="K2" s="2" t="n">
-        <f aca="false">D2</f>
         <v>-0.0446439316594496</v>
       </c>
       <c r="L2" s="2" t="n">
-        <f aca="false">E2</f>
         <v>0.0288080404484257</v>
       </c>
       <c r="M2" s="2" t="n">
-        <f aca="false">F2</f>
         <v>0.0151547090932502</v>
       </c>
       <c r="N2" s="2" t="n">
-        <f aca="false">G2</f>
         <v>0.012055928654588</v>
       </c>
     </row>
@@ -472,29 +529,24 @@
       <c r="G3" s="2" t="n">
         <v>-0.0239034341045996</v>
       </c>
+      <c r="H3" s="3"/>
       <c r="I3" s="2" t="n">
-        <f aca="false">I2+B3</f>
-        <v>-0.0446439316594496</v>
+        <v>0</v>
       </c>
       <c r="J3" s="2" t="n">
-        <f aca="false">J2+C3</f>
-        <v>-0.0412754894569492</v>
+        <v>-0.0700835299053749</v>
       </c>
       <c r="K3" s="2" t="n">
-        <f aca="false">K2+D3</f>
-        <v>-0.0446439316594496</v>
+        <v>0</v>
       </c>
       <c r="L3" s="2" t="n">
-        <f aca="false">L2+E3</f>
-        <v>-0.0412754894569492</v>
+        <v>-0.0700835299053749</v>
       </c>
       <c r="M3" s="2" t="n">
-        <f aca="false">M2+F3</f>
-        <v>-0.133376399481825</v>
+        <v>-0.148531108575075</v>
       </c>
       <c r="N3" s="2" t="n">
-        <f aca="false">N2+G3</f>
-        <v>-0.0118475054500116</v>
+        <v>-0.0239034341045996</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,28 +573,22 @@
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="2" t="n">
-        <f aca="false">I3+B4</f>
-        <v>-0.0534082933669869</v>
+        <v>-0.0353683718975998</v>
       </c>
       <c r="J4" s="2" t="n">
-        <f aca="false">J3+C4</f>
-        <v>0.0307464440428512</v>
+        <v>0.0720219334998004</v>
       </c>
       <c r="K4" s="2" t="n">
-        <f aca="false">K3+D4</f>
-        <v>-0.0534082933669869</v>
+        <v>-0.0353683718975998</v>
       </c>
       <c r="L4" s="2" t="n">
-        <f aca="false">L3+E4</f>
-        <v>0.0195102301794011</v>
+        <v>0.0607857196363503</v>
       </c>
       <c r="M4" s="2" t="n">
-        <f aca="false">M3+F4</f>
-        <v>-0.158943425218087</v>
+        <v>-0.0255670257362622</v>
       </c>
       <c r="N4" s="2" t="n">
-        <f aca="false">N3+G4</f>
-        <v>0.0343971760515015</v>
+        <v>0.0196406713114506</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,29 +613,24 @@
       <c r="G5" s="2" t="n">
         <v>0.00877729296873769</v>
       </c>
+      <c r="H5" s="3"/>
       <c r="I5" s="2" t="n">
-        <f aca="false">I4+B5</f>
-        <v>0.0672122532788631</v>
+        <v>0.0924586279672126</v>
       </c>
       <c r="J5" s="2" t="n">
-        <f aca="false">J4+C5</f>
-        <v>0.135964110013388</v>
+        <v>0.105217665970537</v>
       </c>
       <c r="K5" s="2" t="n">
-        <f aca="false">K4+D5</f>
-        <v>0.0546048455340011</v>
+        <v>0.0735972649489125</v>
       </c>
       <c r="L5" s="2" t="n">
-        <f aca="false">L4+E5</f>
-        <v>0.0174735781398762</v>
+        <v>-0.00203665203952491</v>
       </c>
       <c r="M5" s="2" t="n">
-        <f aca="false">M4+F5</f>
-        <v>-0.0806440726151617</v>
+        <v>0.00828956929462502</v>
       </c>
       <c r="N5" s="2" t="n">
-        <f aca="false">N4+G5</f>
-        <v>0.0431744690202392</v>
+        <v>0.00877729296873769</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,29 +655,24 @@
       <c r="G6" s="2" t="n">
         <v>-0.0619507314979746</v>
       </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="2" t="n">
-        <f aca="false">I5+B6</f>
-        <v>0.345060054177763</v>
+        <v>0.2778478008989</v>
       </c>
       <c r="J6" s="2" t="n">
-        <f aca="false">J5+C6</f>
-        <v>0.426505697428238</v>
+        <v>0.144502246056187</v>
       </c>
       <c r="K6" s="2" t="n">
-        <f aca="false">K5+D6</f>
-        <v>0.248282412207001</v>
+        <v>0.193677566673</v>
       </c>
       <c r="L6" s="2" t="n">
-        <f aca="false">L5+E6</f>
-        <v>0.279521697788676</v>
+        <v>0.116008778290138</v>
       </c>
       <c r="M6" s="2" t="n">
-        <f aca="false">M5+F6</f>
-        <v>-0.0561264154399365</v>
+        <v>0.0245176571752252</v>
       </c>
       <c r="N6" s="2" t="n">
-        <f aca="false">N5+G6</f>
-        <v>-0.0187762624777354</v>
+        <v>-0.164606116063325</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,29 +697,24 @@
       <c r="G7" s="2" t="n">
         <v>-0.094241278495737</v>
       </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="2" t="n">
-        <f aca="false">I6+B7</f>
-        <v>0.218027263723001</v>
+        <v>-0.133597647995575</v>
       </c>
       <c r="J7" s="2" t="n">
-        <f aca="false">J6+C7</f>
-        <v>0.415646460178314</v>
+        <v>-0.010859237249924</v>
       </c>
       <c r="K7" s="2" t="n">
-        <f aca="false">K6+D7</f>
-        <v>0.0977271076597391</v>
+        <v>-0.157120162088075</v>
       </c>
       <c r="L7" s="2" t="n">
-        <f aca="false">L6+E7</f>
-        <v>0.327706706201865</v>
+        <v>0.0315515362577509</v>
       </c>
       <c r="M7" s="2" t="n">
-        <f aca="false">M6+F7</f>
-        <v>-0.142784592863761</v>
+        <v>-0.0783822658152621</v>
       </c>
       <c r="N7" s="2" t="n">
-        <f aca="false">N6+G7</f>
-        <v>-0.113017540973472</v>
+        <v>-0.094241278495737</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,29 +739,24 @@
       <c r="G8" s="2" t="n">
         <v>-0.1682060420022</v>
       </c>
+      <c r="H8" s="3"/>
       <c r="I8" s="2" t="n">
-        <f aca="false">I7+B8</f>
-        <v>0.0632462028616391</v>
+        <v>-0.127355715338512</v>
       </c>
       <c r="J8" s="2" t="n">
-        <f aca="false">J7+C8</f>
-        <v>0.248318297747102</v>
+        <v>-0.167328162431212</v>
       </c>
       <c r="K8" s="2" t="n">
-        <f aca="false">K7+D8</f>
-        <v>-0.0660104614008859</v>
+        <v>-0.163737569060625</v>
       </c>
       <c r="L8" s="2" t="n">
-        <f aca="false">L7+E8</f>
-        <v>0.160378543770653</v>
+        <v>-0.167328162431212</v>
       </c>
       <c r="M8" s="2" t="n">
-        <f aca="false">M7+F8</f>
-        <v>-0.327770859174848</v>
+        <v>-0.0333737132211373</v>
       </c>
       <c r="N8" s="2" t="n">
-        <f aca="false">N7+G8</f>
-        <v>-0.281223582975672</v>
+        <v>-0.0356581606294873</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,29 +781,24 @@
       <c r="G9" s="2" t="n">
         <v>0.00294571552728759</v>
       </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="2" t="n">
-        <f aca="false">I8+B9</f>
-        <v>0.0533011822824264</v>
+        <v>-0.0166911896484751</v>
       </c>
       <c r="J9" s="2" t="n">
-        <f aca="false">J8+C9</f>
-        <v>0.24715460295289</v>
+        <v>-0.00790986386347484</v>
       </c>
       <c r="K9" s="2" t="n">
-        <f aca="false">K8+D9</f>
-        <v>-0.0535672304175859</v>
+        <v>0.00415815586308743</v>
       </c>
       <c r="L9" s="2" t="n">
-        <f aca="false">L8+E9</f>
-        <v>0.15828190719834</v>
+        <v>-0.00884280564157494</v>
       </c>
       <c r="M9" s="2" t="n">
-        <f aca="false">M8+F9</f>
-        <v>-0.326003930494035</v>
+        <v>0.0017669286808126</v>
       </c>
       <c r="N9" s="2" t="n">
-        <f aca="false">N8+G9</f>
-        <v>-0.278277867448385</v>
+        <v>0.00294571552728759</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,29 +823,24 @@
       <c r="G10" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="H10" s="3"/>
       <c r="I10" s="2" t="n">
-        <f aca="false">I9+B10</f>
-        <v>0.0533011822824264</v>
+        <v>0</v>
       </c>
       <c r="J10" s="2" t="n">
-        <f aca="false">J9+C10</f>
-        <v>0.24715460295289</v>
+        <v>0</v>
       </c>
       <c r="K10" s="2" t="n">
-        <f aca="false">K9+D10</f>
-        <v>-0.0535672304175859</v>
+        <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <f aca="false">L9+E10</f>
-        <v>0.15828190719834</v>
+        <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <f aca="false">M9+F10</f>
-        <v>-0.37360246081761</v>
+        <v>-0.0475985303235747</v>
       </c>
       <c r="N10" s="2" t="n">
-        <f aca="false">N9+G10</f>
-        <v>-0.278277867448385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -849,29 +865,24 @@
       <c r="G11" s="2" t="n">
         <v>-0.0493539649890125</v>
       </c>
+      <c r="H11" s="3"/>
       <c r="I11" s="2" t="n">
-        <f aca="false">I10+B11</f>
-        <v>0.00783253905322679</v>
+        <v>-0.0454686432291996</v>
       </c>
       <c r="J11" s="2" t="n">
-        <f aca="false">J10+C11</f>
-        <v>0.19574739292689</v>
+        <v>-0.0684153861603248</v>
       </c>
       <c r="K11" s="2" t="n">
-        <f aca="false">K10+D11</f>
-        <v>-0.0990358736467855</v>
+        <v>-0.0454686432291996</v>
       </c>
       <c r="L11" s="2" t="n">
-        <f aca="false">L10+E11</f>
-        <v>0.0860125345909153</v>
+        <v>-0.0989201987454871</v>
       </c>
       <c r="M11" s="2" t="n">
-        <f aca="false">M10+F11</f>
-        <v>-0.421835055621822</v>
+        <v>-0.0535544012870747</v>
       </c>
       <c r="N11" s="2" t="n">
-        <f aca="false">N10+G11</f>
-        <v>-0.327631832437397</v>
+        <v>-0.0493539649890125</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,29 +907,24 @@
       <c r="G12" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="2" t="n">
-        <f aca="false">I11+B12</f>
-        <v>0.00783253905322679</v>
+        <v>0</v>
       </c>
       <c r="J12" s="2" t="n">
-        <f aca="false">J11+C12</f>
-        <v>0.207324805827515</v>
+        <v>0.0115774129006252</v>
       </c>
       <c r="K12" s="2" t="n">
-        <f aca="false">K11+D12</f>
-        <v>-0.0990358736467855</v>
+        <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <f aca="false">L11+E12</f>
-        <v>0.101502446419816</v>
+        <v>0.0154899118289003</v>
       </c>
       <c r="M12" s="2" t="n">
-        <f aca="false">M11+F12</f>
-        <v>-0.407584771336972</v>
+        <v>0.0142502842848502</v>
       </c>
       <c r="N12" s="2" t="n">
-        <f aca="false">N11+G12</f>
-        <v>-0.327631832437397</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -943,29 +949,24 @@
       <c r="G13" s="2" t="n">
         <v>-0.0538636614733498</v>
       </c>
+      <c r="H13" s="3"/>
       <c r="I13" s="2" t="n">
-        <f aca="false">I12+B13</f>
-        <v>-0.0319901798069482</v>
+        <v>-0.039822718860175</v>
       </c>
       <c r="J13" s="2" t="n">
-        <f aca="false">J12+C13</f>
-        <v>0.218825920761391</v>
+        <v>0.0115011149338753</v>
       </c>
       <c r="K13" s="2" t="n">
-        <f aca="false">K12+D13</f>
-        <v>-0.138858592506961</v>
+        <v>-0.039822718860175</v>
       </c>
       <c r="L13" s="2" t="n">
-        <f aca="false">L12+E13</f>
-        <v>0.101502446419816</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <f aca="false">M12+F13</f>
-        <v>-0.450898265092022</v>
+        <v>-0.0433134937550496</v>
       </c>
       <c r="N13" s="2" t="n">
-        <f aca="false">N12+G13</f>
-        <v>-0.381495493910747</v>
+        <v>-0.0538636614733498</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,29 +991,24 @@
       <c r="G14" s="2" t="n">
         <v>0.0362524098707251</v>
       </c>
+      <c r="H14" s="3"/>
       <c r="I14" s="2" t="n">
-        <f aca="false">I13+B14</f>
-        <v>-0.0395529687642979</v>
+        <v>-0.0249966164062748</v>
       </c>
       <c r="J14" s="2" t="n">
-        <f aca="false">J13+C14</f>
-        <v>0.231608491644841</v>
+        <v>-0.01040740792765</v>
       </c>
       <c r="K14" s="2" t="n">
-        <f aca="false">K13+D14</f>
-        <v>-0.140743350404635</v>
+        <v>-0.0193185853465997</v>
       </c>
       <c r="L14" s="2" t="n">
-        <f aca="false">L13+E14</f>
-        <v>0.12121800314059</v>
+        <v>-0.0034744220903252</v>
       </c>
       <c r="M14" s="2" t="n">
-        <f aca="false">M13+F14</f>
-        <v>-0.429957781903922</v>
+        <v>0.000568273422474987</v>
       </c>
       <c r="N14" s="2" t="n">
-        <f aca="false">N13+G14</f>
-        <v>-0.345243084040022</v>
+        <v>0.0130624310596251</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,29 +1033,24 @@
       <c r="G15" s="2" t="n">
         <v>0.0410639189503002</v>
       </c>
+      <c r="H15" s="3"/>
       <c r="I15" s="2" t="n">
-        <f aca="false">I14+B15</f>
-        <v>-0.026129626091023</v>
+        <v>0.0182128647385749</v>
       </c>
       <c r="J15" s="2" t="n">
-        <f aca="false">J14+C15</f>
-        <v>0.25117231791689</v>
+        <v>0.021351996479375</v>
       </c>
       <c r="K15" s="2" t="n">
-        <f aca="false">K14+D15</f>
-        <v>-0.12732000773136</v>
+        <v>0.0182128647385749</v>
       </c>
       <c r="L15" s="2" t="n">
-        <f aca="false">L14+E15</f>
-        <v>0.13688153743044</v>
+        <v>0.017451704497175</v>
       </c>
       <c r="M15" s="2" t="n">
-        <f aca="false">M14+F15</f>
-        <v>-0.398945894979872</v>
+        <v>0.03692636280045</v>
       </c>
       <c r="N15" s="2" t="n">
-        <f aca="false">N14+G15</f>
-        <v>-0.304179165089722</v>
+        <v>0.0410639189503002</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,29 +1075,24 @@
       <c r="G16" s="2" t="n">
         <v>-0.0100291173878746</v>
       </c>
+      <c r="H16" s="3"/>
       <c r="I16" s="2" t="n">
-        <f aca="false">I15+B16</f>
-        <v>-0.0433103685689976</v>
+        <v>-0.0171807424779746</v>
       </c>
       <c r="J16" s="2" t="n">
-        <f aca="false">J15+C16</f>
-        <v>0.208690815558091</v>
+        <v>-0.0433299071314249</v>
       </c>
       <c r="K16" s="2" t="n">
-        <f aca="false">K15+D16</f>
-        <v>-0.136900687418885</v>
+        <v>-0.0095806796875246</v>
       </c>
       <c r="L16" s="2" t="n">
-        <f aca="false">L15+E16</f>
-        <v>0.0871405811704403</v>
+        <v>-0.0437731834034251</v>
       </c>
       <c r="M16" s="2" t="n">
-        <f aca="false">M15+F16</f>
-        <v>-0.417834359032397</v>
+        <v>-0.0048320042868998</v>
       </c>
       <c r="N16" s="2" t="n">
-        <f aca="false">N15+G16</f>
-        <v>-0.314208282477596</v>
+        <v>-0.00578212012224961</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,29 +1117,24 @@
       <c r="G17" s="2" t="n">
         <v>-0.00614838339849955</v>
       </c>
+      <c r="H17" s="3"/>
       <c r="I17" s="2" t="n">
-        <f aca="false">I16+B17</f>
-        <v>-0.0327061268772977</v>
+        <v>0.0106042416916999</v>
       </c>
       <c r="J17" s="2" t="n">
-        <f aca="false">J16+C17</f>
-        <v>0.220878652667441</v>
+        <v>0.0121878371093501</v>
       </c>
       <c r="K17" s="2" t="n">
-        <f aca="false">K16+D17</f>
-        <v>-0.12897320295376</v>
+        <v>0.00792748446512503</v>
       </c>
       <c r="L17" s="2" t="n">
-        <f aca="false">L16+E17</f>
-        <v>0.0939082166271403</v>
+        <v>0.0067676354567</v>
       </c>
       <c r="M17" s="2" t="n">
-        <f aca="false">M16+F17</f>
-        <v>-0.408605818778096</v>
+        <v>0.0118113092046251</v>
       </c>
       <c r="N17" s="2" t="n">
-        <f aca="false">N16+G17</f>
-        <v>-0.320356665876096</v>
+        <v>-0.00356561444817473</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,29 +1159,24 @@
       <c r="G18" s="2" t="n">
         <v>-4.16333634234434E-017</v>
       </c>
+      <c r="H18" s="3"/>
       <c r="I18" s="2" t="n">
-        <f aca="false">I17+B18</f>
-        <v>-0.00988647649167269</v>
+        <v>0.0194980467748501</v>
       </c>
       <c r="J18" s="2" t="n">
-        <f aca="false">J17+C18</f>
-        <v>0.220878652667441</v>
+        <v>-4.16333634234434E-017</v>
       </c>
       <c r="K18" s="2" t="n">
-        <f aca="false">K17+D18</f>
-        <v>-0.106153552568135</v>
+        <v>0.0194980467748501</v>
       </c>
       <c r="L18" s="2" t="n">
-        <f aca="false">L17+E18</f>
-        <v>0.0939082166271402</v>
+        <v>-4.16333634234434E-017</v>
       </c>
       <c r="M18" s="2" t="n">
-        <f aca="false">M17+F18</f>
-        <v>-0.400224292215596</v>
+        <v>4.16333634234434E-017</v>
       </c>
       <c r="N18" s="2" t="n">
-        <f aca="false">N17+G18</f>
-        <v>-0.320356665876096</v>
+        <v>-4.16333634234434E-017</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1225,29 +1201,24 @@
       <c r="G19" s="2" t="n">
         <v>0.0251885801782501</v>
       </c>
+      <c r="H19" s="3"/>
       <c r="I19" s="2" t="n">
-        <f aca="false">I18+B19</f>
-        <v>-0.00369906360609773</v>
+        <v>0.0168958748046502</v>
       </c>
       <c r="J19" s="2" t="n">
-        <f aca="false">J18+C19</f>
-        <v>0.224440807845691</v>
+        <v>0.0142706170973252</v>
       </c>
       <c r="K19" s="2" t="n">
-        <f aca="false">K18+D19</f>
-        <v>-0.0999661396825598</v>
+        <v>0.0168958748046502</v>
       </c>
       <c r="L19" s="2" t="n">
-        <f aca="false">L18+E19</f>
-        <v>0.106891486539015</v>
+        <v>0.02369173183095</v>
       </c>
       <c r="M19" s="2" t="n">
-        <f aca="false">M18+F19</f>
-        <v>-0.362906664481296</v>
+        <v>0.0480260896533753</v>
       </c>
       <c r="N19" s="2" t="n">
-        <f aca="false">N18+G19</f>
-        <v>-0.295168085697846</v>
+        <v>0.0251885801782501</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,29 +1243,24 @@
       <c r="G20" s="2" t="n">
         <v>0.0410770820361752</v>
       </c>
+      <c r="H20" s="3"/>
       <c r="I20" s="2" t="n">
-        <f aca="false">I19+B20</f>
-        <v>-0.0615127925173976</v>
+        <v>-0.0578137289112999</v>
       </c>
       <c r="J20" s="2" t="n">
-        <f aca="false">J19+C20</f>
-        <v>0.253609557460041</v>
+        <v>0.02916874961435</v>
       </c>
       <c r="K20" s="2" t="n">
-        <f aca="false">K19+D20</f>
-        <v>-0.15777986859386</v>
+        <v>-0.0578137289112999</v>
       </c>
       <c r="L20" s="2" t="n">
-        <f aca="false">L19+E20</f>
-        <v>0.136060236153365</v>
+        <v>0.02916874961435</v>
       </c>
       <c r="M20" s="2" t="n">
-        <f aca="false">M19+F20</f>
-        <v>-0.399810250113421</v>
+        <v>-0.0369035856321249</v>
       </c>
       <c r="N20" s="2" t="n">
-        <f aca="false">N19+G20</f>
-        <v>-0.254091003661671</v>
+        <v>0.0410770820361752</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,29 +1285,24 @@
       <c r="G21" s="2" t="n">
         <v>-0.0244403402493499</v>
       </c>
+      <c r="H21" s="3"/>
       <c r="I21" s="2" t="n">
-        <f aca="false">I20+B21</f>
-        <v>-0.0969910475204223</v>
+        <v>-0.0354782550030247</v>
       </c>
       <c r="J21" s="2" t="n">
-        <f aca="false">J20+C21</f>
-        <v>0.240318550624116</v>
+        <v>-0.0132910068359245</v>
       </c>
       <c r="K21" s="2" t="n">
-        <f aca="false">K20+D21</f>
-        <v>-0.193258123596884</v>
+        <v>-0.0354782550030247</v>
       </c>
       <c r="L21" s="2" t="n">
-        <f aca="false">L20+E21</f>
-        <v>0.124228858113491</v>
+        <v>-0.0118313780398745</v>
       </c>
       <c r="M21" s="2" t="n">
-        <f aca="false">M20+F21</f>
-        <v>-0.416705308141271</v>
+        <v>-0.0168950580278498</v>
       </c>
       <c r="N21" s="2" t="n">
-        <f aca="false">N20+G21</f>
-        <v>-0.278531343911021</v>
+        <v>-0.0110255588090499</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1366,29 +1327,24 @@
       <c r="G22" s="2" t="n">
         <v>0.0157138250000002</v>
       </c>
+      <c r="H22" s="3"/>
       <c r="I22" s="2" t="n">
-        <f aca="false">I21+B22</f>
-        <v>-0.0698042719294971</v>
+        <v>0.0271867755909252</v>
       </c>
       <c r="J22" s="2" t="n">
-        <f aca="false">J21+C22</f>
-        <v>0.258437250523941</v>
+        <v>0.0181186998998251</v>
       </c>
       <c r="K22" s="2" t="n">
-        <f aca="false">K21+D22</f>
-        <v>-0.157764467627359</v>
+        <v>0.0354936559695254</v>
       </c>
       <c r="L22" s="2" t="n">
-        <f aca="false">L21+E22</f>
-        <v>0.150266895913966</v>
+        <v>0.0260380378004752</v>
       </c>
       <c r="M22" s="2" t="n">
-        <f aca="false">M21+F22</f>
-        <v>-0.401847969369246</v>
+        <v>0.0148573387720252</v>
       </c>
       <c r="N22" s="2" t="n">
-        <f aca="false">N21+G22</f>
-        <v>-0.26281751891102</v>
+        <v>0.0157138250000002</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,29 +1369,24 @@
       <c r="G23" s="2" t="n">
         <v>-0.0156034069361249</v>
       </c>
+      <c r="H23" s="3"/>
       <c r="I23" s="2" t="n">
-        <f aca="false">I22+B23</f>
-        <v>-0.0731941365729468</v>
+        <v>-0.00338986464344965</v>
       </c>
       <c r="J23" s="2" t="n">
-        <f aca="false">J22+C23</f>
-        <v>0.253176127777517</v>
+        <v>-0.0132018234325246</v>
       </c>
       <c r="K23" s="2" t="n">
-        <f aca="false">K22+D23</f>
-        <v>-0.161343857270809</v>
+        <v>-0.00357938964344956</v>
       </c>
       <c r="L23" s="2" t="n">
-        <f aca="false">L22+E23</f>
-        <v>0.153577626973641</v>
+        <v>0.00331073105967511</v>
       </c>
       <c r="M23" s="2" t="n">
-        <f aca="false">M22+F23</f>
-        <v>-0.41434374515052</v>
+        <v>-0.0124957757812745</v>
       </c>
       <c r="N23" s="2" t="n">
-        <f aca="false">N22+G23</f>
-        <v>-0.278420925847145</v>
+        <v>-0.0133737451222249</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1460,29 +1411,24 @@
       <c r="G24" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="H24" s="3"/>
       <c r="I24" s="2" t="n">
-        <f aca="false">I23+B24</f>
-        <v>-0.0731941365729468</v>
+        <v>0</v>
       </c>
       <c r="J24" s="2" t="n">
-        <f aca="false">J23+C24</f>
-        <v>0.253176127777517</v>
+        <v>0</v>
       </c>
       <c r="K24" s="2" t="n">
-        <f aca="false">K23+D24</f>
-        <v>-0.161343857270809</v>
+        <v>0</v>
       </c>
       <c r="L24" s="2" t="n">
-        <f aca="false">L23+E24</f>
-        <v>0.153577626973641</v>
+        <v>0</v>
       </c>
       <c r="M24" s="2" t="n">
-        <f aca="false">M23+F24</f>
-        <v>-0.41434374515052</v>
+        <v>0</v>
       </c>
       <c r="N24" s="2" t="n">
-        <f aca="false">N23+G24</f>
-        <v>-0.278420925847145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1507,29 +1453,24 @@
       <c r="G25" s="2" t="n">
         <v>0.0132804041015502</v>
       </c>
+      <c r="H25" s="3"/>
       <c r="I25" s="2" t="n">
-        <f aca="false">I24+B25</f>
-        <v>-0.0389739819906215</v>
+        <v>0.0342201545823253</v>
       </c>
       <c r="J25" s="2" t="n">
-        <f aca="false">J24+C25</f>
-        <v>0.275538457660317</v>
+        <v>0.0223623298828002</v>
       </c>
       <c r="K25" s="2" t="n">
-        <f aca="false">K24+D25</f>
-        <v>-0.223807389101783</v>
+        <v>-0.0624635318309745</v>
       </c>
       <c r="L25" s="2" t="n">
-        <f aca="false">L24+E25</f>
-        <v>0.0800323290268911</v>
+        <v>-0.0735452979467498</v>
       </c>
       <c r="M25" s="2" t="n">
-        <f aca="false">M24+F25</f>
-        <v>-0.392623380792545</v>
+        <v>0.0217203643579751</v>
       </c>
       <c r="N25" s="2" t="n">
-        <f aca="false">N24+G25</f>
-        <v>-0.265140521745595</v>
+        <v>0.0132804041015502</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,29 +1495,24 @@
       <c r="G26" s="2" t="n">
         <v>-0.026756889358</v>
       </c>
+      <c r="H26" s="3"/>
       <c r="I26" s="2" t="n">
-        <f aca="false">I25+B26</f>
-        <v>-0.0556570544615715</v>
+        <v>-0.01668307247095</v>
       </c>
       <c r="J26" s="2" t="n">
-        <f aca="false">J25+C26</f>
-        <v>0.262751782364792</v>
+        <v>-0.000578026657699696</v>
       </c>
       <c r="K26" s="2" t="n">
-        <f aca="false">K25+D26</f>
-        <v>-0.250370615584158</v>
+        <v>-0.0265632264823748</v>
       </c>
       <c r="L26" s="2" t="n">
-        <f aca="false">L25+E26</f>
-        <v>0.0663417468754662</v>
+        <v>-0.00148193351359995</v>
       </c>
       <c r="M26" s="2" t="n">
-        <f aca="false">M25+F26</f>
-        <v>-0.400532575989945</v>
+        <v>-0.0079091951973996</v>
       </c>
       <c r="N26" s="2" t="n">
-        <f aca="false">N25+G26</f>
-        <v>-0.291897411103595</v>
+        <v>-0.026756889358</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,29 +1537,24 @@
       <c r="G27" s="2" t="n">
         <v>-0.00118681091254976</v>
       </c>
+      <c r="H27" s="3"/>
       <c r="I27" s="2" t="n">
-        <f aca="false">I26+B27</f>
-        <v>-0.0455332830774214</v>
+        <v>0.0101237713841501</v>
       </c>
       <c r="J27" s="2" t="n">
-        <f aca="false">J26+C27</f>
-        <v>0.265056575924442</v>
+        <v>0.00859109512215023</v>
       </c>
       <c r="K27" s="2" t="n">
-        <f aca="false">K26+D27</f>
-        <v>-0.254706384128883</v>
+        <v>-0.00433576854472503</v>
       </c>
       <c r="L27" s="2" t="n">
-        <f aca="false">L26+E27</f>
-        <v>0.0738257084940412</v>
+        <v>0.0137702631810751</v>
       </c>
       <c r="M27" s="2" t="n">
-        <f aca="false">M26+F27</f>
-        <v>-0.403562971197319</v>
+        <v>0.00325590635512524</v>
       </c>
       <c r="N27" s="2" t="n">
-        <f aca="false">N26+G27</f>
-        <v>-0.293084222016145</v>
+        <v>0.00573306281040023</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1648,29 +1579,24 @@
       <c r="G28" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="H28" s="3"/>
       <c r="I28" s="2" t="n">
-        <f aca="false">I27+B28</f>
-        <v>-0.0455332830774214</v>
+        <v>0</v>
       </c>
       <c r="J28" s="2" t="n">
-        <f aca="false">J27+C28</f>
-        <v>0.265056575924442</v>
+        <v>0</v>
       </c>
       <c r="K28" s="2" t="n">
-        <f aca="false">K27+D28</f>
-        <v>-0.254706384128883</v>
+        <v>0</v>
       </c>
       <c r="L28" s="2" t="n">
-        <f aca="false">L27+E28</f>
-        <v>0.0738257084940412</v>
+        <v>0</v>
       </c>
       <c r="M28" s="2" t="n">
-        <f aca="false">M27+F28</f>
-        <v>-0.387705156639044</v>
+        <v>0.0158578145582751</v>
       </c>
       <c r="N28" s="2" t="n">
-        <f aca="false">N27+G28</f>
-        <v>-0.293084222016145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,29 +1621,24 @@
       <c r="G29" s="2" t="n">
         <v>0.00963957168467526</v>
       </c>
+      <c r="H29" s="3"/>
       <c r="I29" s="2" t="n">
-        <f aca="false">I28+B29</f>
-        <v>-0.0584471079872714</v>
+        <v>-0.0154022961939</v>
       </c>
       <c r="J29" s="2" t="n">
-        <f aca="false">J28+C29</f>
-        <v>0.260745661471317</v>
+        <v>-0.00431091445312511</v>
       </c>
       <c r="K29" s="2" t="n">
-        <f aca="false">K28+D29</f>
-        <v>-0.267620209038733</v>
+        <v>-0.0154022961939</v>
       </c>
       <c r="L29" s="2" t="n">
-        <f aca="false">L28+E29</f>
-        <v>0.0695147940409161</v>
+        <v>-0.00431091445312511</v>
       </c>
       <c r="M29" s="2" t="n">
-        <f aca="false">M28+F29</f>
-        <v>-0.397109625784669</v>
+        <v>-0.00393728056890004</v>
       </c>
       <c r="N29" s="2" t="n">
-        <f aca="false">N28+G29</f>
-        <v>-0.28344465033147</v>
+        <v>0.00963957168467526</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,29 +1663,24 @@
       <c r="G30" s="2" t="n">
         <v>0.020174827043275</v>
       </c>
+      <c r="H30" s="3"/>
       <c r="I30" s="2" t="n">
-        <f aca="false">I29+B30</f>
-        <v>-0.0511191456775964</v>
+        <v>0.00732796230967501</v>
       </c>
       <c r="J30" s="2" t="n">
-        <f aca="false">J29+C30</f>
-        <v>0.268073623780992</v>
+        <v>0.00732796230967501</v>
       </c>
       <c r="K30" s="2" t="n">
-        <f aca="false">K29+D30</f>
-        <v>-0.266041860110458</v>
+        <v>0.00157834892827511</v>
       </c>
       <c r="L30" s="2" t="n">
-        <f aca="false">L29+E30</f>
-        <v>0.0768427563505911</v>
+        <v>0.00732796230967501</v>
       </c>
       <c r="M30" s="2" t="n">
-        <f aca="false">M29+F30</f>
-        <v>-0.395531276856394</v>
+        <v>0.00157834892827511</v>
       </c>
       <c r="N30" s="2" t="n">
-        <f aca="false">N29+G30</f>
-        <v>-0.263269823288195</v>
+        <v>0.016205827729375</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1789,29 +1705,24 @@
       <c r="G31" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="H31" s="3"/>
       <c r="I31" s="2" t="n">
-        <f aca="false">I30+B31</f>
-        <v>-0.0511191456775964</v>
+        <v>0</v>
       </c>
       <c r="J31" s="2" t="n">
-        <f aca="false">J30+C31</f>
-        <v>0.283473250438667</v>
+        <v>0.015399626657675</v>
       </c>
       <c r="K31" s="2" t="n">
-        <f aca="false">K30+D31</f>
-        <v>-0.266041860110458</v>
+        <v>0</v>
       </c>
       <c r="L31" s="2" t="n">
-        <f aca="false">L30+E31</f>
-        <v>0.0922313398391912</v>
+        <v>0.0153885834886001</v>
       </c>
       <c r="M31" s="2" t="n">
-        <f aca="false">M30+F31</f>
-        <v>-0.380142693367794</v>
+        <v>0.0153885834886001</v>
       </c>
       <c r="N31" s="2" t="n">
-        <f aca="false">N30+G31</f>
-        <v>-0.263269823288195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,29 +1747,24 @@
       <c r="G32" s="2" t="n">
         <v>-0.0118542398487502</v>
       </c>
+      <c r="H32" s="3"/>
       <c r="I32" s="2" t="n">
-        <f aca="false">I31+B32</f>
-        <v>-0.0475174693054212</v>
+        <v>0.0036016763721752</v>
       </c>
       <c r="J32" s="2" t="n">
-        <f aca="false">J31+C32</f>
-        <v>0.271619010589917</v>
+        <v>0</v>
       </c>
       <c r="K32" s="2" t="n">
-        <f aca="false">K31+D32</f>
-        <v>-0.263269901126083</v>
+        <v>0.00277195898437518</v>
       </c>
       <c r="L32" s="2" t="n">
-        <f aca="false">L31+E32</f>
-        <v>0.080377099990441</v>
+        <v>0</v>
       </c>
       <c r="M32" s="2" t="n">
-        <f aca="false">M31+F32</f>
-        <v>-0.373412767396244</v>
+        <v>0.0129494203125</v>
       </c>
       <c r="N32" s="2" t="n">
-        <f aca="false">N31+G32</f>
-        <v>-0.275124063136945</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,29 +1789,24 @@
       <c r="G33" s="2" t="n">
         <v>0.0443855028395253</v>
       </c>
+      <c r="H33" s="3"/>
       <c r="I33" s="2" t="n">
-        <f aca="false">I32+B33</f>
-        <v>-0.024183191270571</v>
+        <v>0.0357134299879752</v>
       </c>
       <c r="J33" s="2" t="n">
-        <f aca="false">J32+C33</f>
-        <v>0.266038818302267</v>
+        <v>-0.00558019228764981</v>
       </c>
       <c r="K33" s="2" t="n">
-        <f aca="false">K32+D33</f>
-        <v>-0.254842343108257</v>
+        <v>0.031378973147025</v>
       </c>
       <c r="L33" s="2" t="n">
-        <f aca="false">L32+E33</f>
-        <v>0.0747969077027912</v>
+        <v>-0.00558019228764981</v>
       </c>
       <c r="M33" s="2" t="n">
-        <f aca="false">M32+F33</f>
-        <v>-0.336741490543294</v>
+        <v>0.0443899002904502</v>
       </c>
       <c r="N33" s="2" t="n">
-        <f aca="false">N32+G33</f>
-        <v>-0.230738560297419</v>
+        <v>0.0443855028395253</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,29 +1831,24 @@
       <c r="G34" s="2" t="n">
         <v>0.0163769066306248</v>
       </c>
+      <c r="H34" s="3"/>
       <c r="I34" s="2" t="n">
-        <f aca="false">I33+B34</f>
-        <v>-0.026082536007121</v>
+        <v>-0.00189934473655003</v>
       </c>
       <c r="J34" s="2" t="n">
-        <f aca="false">J33+C34</f>
-        <v>0.256311992626167</v>
+        <v>-0.0016847785056249</v>
       </c>
       <c r="K34" s="2" t="n">
-        <f aca="false">K33+D34</f>
-        <v>-0.253286789697782</v>
+        <v>0.00155555341047501</v>
       </c>
       <c r="L34" s="2" t="n">
-        <f aca="false">L33+E34</f>
-        <v>0.0674672790970163</v>
+        <v>-0.00689730048077482</v>
       </c>
       <c r="M34" s="2" t="n">
-        <f aca="false">M33+F34</f>
-        <v>-0.340194922279094</v>
+        <v>-0.00302110361080028</v>
       </c>
       <c r="N34" s="2" t="n">
-        <f aca="false">N33+G34</f>
-        <v>-0.214361653666795</v>
+        <v>-0.0134828299929751</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1977,29 +1873,24 @@
       <c r="G35" s="2" t="n">
         <v>-0.0988360378856248</v>
       </c>
+      <c r="H35" s="3"/>
       <c r="I35" s="2" t="n">
-        <f aca="false">I34+B35</f>
-        <v>-0.117474187374296</v>
+        <v>0.0104879138622001</v>
       </c>
       <c r="J35" s="2" t="n">
-        <f aca="false">J34+C35</f>
-        <v>0.161121765277392</v>
+        <v>1.38777878078145E-017</v>
       </c>
       <c r="K35" s="2" t="n">
-        <f aca="false">K34+D35</f>
-        <v>-0.345642252488257</v>
+        <v>5.55111512312578E-017</v>
       </c>
       <c r="L35" s="2" t="n">
-        <f aca="false">L34+E35</f>
-        <v>-0.0277229482517586</v>
+        <v>1.38777878078145E-017</v>
       </c>
       <c r="M35" s="2" t="n">
-        <f aca="false">M34+F35</f>
-        <v>-0.419069142391319</v>
+        <v>-0.0788742201122247</v>
       </c>
       <c r="N35" s="2" t="n">
-        <f aca="false">N34+G35</f>
-        <v>-0.313197691552419</v>
+        <v>4.16333634234434E-017</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,115 +1915,182 @@
       <c r="G36" s="2" t="n">
         <v>-0.0309803132712996</v>
       </c>
+      <c r="H36" s="3"/>
       <c r="I36" s="2" t="n">
-        <f aca="false">I35+B36</f>
-        <v>-0.167679069215246</v>
+        <v>-0.0502048818409498</v>
       </c>
       <c r="J36" s="2" t="n">
-        <f aca="false">J35+C36</f>
-        <v>0.112848286751717</v>
+        <v>-0.0444852424829998</v>
       </c>
       <c r="K36" s="2" t="n">
-        <f aca="false">K35+D36</f>
-        <v>-0.375638875144532</v>
+        <v>-0.0299966226562747</v>
       </c>
       <c r="L36" s="2" t="n">
-        <f aca="false">L35+E36</f>
-        <v>-0.0759964267774335</v>
+        <v>-0.0444852424829998</v>
       </c>
       <c r="M36" s="2" t="n">
-        <f aca="false">M35+F36</f>
-        <v>-0.446128968943868</v>
+        <v>-0.0423810810497495</v>
       </c>
       <c r="N36" s="2" t="n">
-        <f aca="false">N35+G36</f>
-        <v>-0.344178004823719</v>
+        <v>-0.0463015677684996</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="3" t="n">
+      <c r="B38" s="4" t="n">
         <f aca="false">AVERAGE(B2:B36)</f>
         <v>-0.00479083054900702</v>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="4" t="n">
         <f aca="false">AVERAGE(C2:C36)</f>
         <v>0.00322423676433478</v>
       </c>
-      <c r="D38" s="3" t="n">
+      <c r="D38" s="4" t="n">
         <f aca="false">AVERAGE(D2:D36)</f>
         <v>-0.0107325392898438</v>
       </c>
-      <c r="E38" s="3" t="n">
+      <c r="E38" s="4" t="n">
         <f aca="false">AVERAGE(E2:E36)</f>
         <v>-0.00217132647935524</v>
       </c>
-      <c r="F38" s="3" t="n">
+      <c r="F38" s="4" t="n">
         <f aca="false">AVERAGE(F2:F36)</f>
         <v>-0.0127465419698248</v>
       </c>
-      <c r="G38" s="3" t="n">
+      <c r="G38" s="4" t="n">
         <f aca="false">AVERAGE(G2:G36)</f>
         <v>-0.00983365728067769</v>
+      </c>
+      <c r="I38" s="4" t="n">
+        <f aca="false">AVERAGE(I2:I36)</f>
+        <v>-0.00290908229565842</v>
+      </c>
+      <c r="J38" s="4" t="n">
+        <f aca="false">AVERAGE(J2:J36)</f>
+        <v>0.00174119567591551</v>
+      </c>
+      <c r="K38" s="4" t="n">
+        <f aca="false">AVERAGE(K2:K36)</f>
+        <v>-0.00982707806821128</v>
+      </c>
+      <c r="L38" s="4" t="n">
+        <f aca="false">AVERAGE(L2:L36)</f>
+        <v>-0.00420090936461308</v>
+      </c>
+      <c r="M38" s="4" t="n">
+        <f aca="false">AVERAGE(M2:M36)</f>
+        <v>-0.00989317092307839</v>
+      </c>
+      <c r="N38" s="4" t="n">
+        <f aca="false">AVERAGE(N2:N36)</f>
+        <v>-0.00780414647213555</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="3" t="n">
+      <c r="B39" s="4" t="n">
         <f aca="false">STDEV(B2:B36)</f>
         <v>0.0678718634319328</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="4" t="n">
         <f aca="false">STDEV(C2:C36)</f>
         <v>0.0672153405120472</v>
       </c>
-      <c r="D39" s="3" t="n">
+      <c r="D39" s="4" t="n">
         <f aca="false">STDEV(D2:D36)</f>
         <v>0.0597982134138702</v>
       </c>
-      <c r="E39" s="3" t="n">
+      <c r="E39" s="4" t="n">
         <f aca="false">STDEV(E2:E36)</f>
         <v>0.063318340862346</v>
       </c>
-      <c r="F39" s="3" t="n">
+      <c r="F39" s="4" t="n">
         <f aca="false">STDEV(F2:F36)</f>
         <v>0.0506432990351529</v>
       </c>
-      <c r="G39" s="3" t="n">
+      <c r="G39" s="4" t="n">
         <f aca="false">STDEV(G2:G36)</f>
         <v>0.044376513171941</v>
+      </c>
+      <c r="I39" s="4" t="n">
+        <f aca="false">STDEV(I2:I36)</f>
+        <v>0.0641327513472022</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <f aca="false">STDEV(J2:J36)</f>
+        <v>0.0494442606826822</v>
+      </c>
+      <c r="K39" s="4" t="n">
+        <f aca="false">STDEV(K2:K36)</f>
+        <v>0.0574246646900162</v>
+      </c>
+      <c r="L39" s="4" t="n">
+        <f aca="false">STDEV(L2:L36)</f>
+        <v>0.0466102758637179</v>
+      </c>
+      <c r="M39" s="4" t="n">
+        <f aca="false">STDEV(M2:M36)</f>
+        <v>0.0390082166089497</v>
+      </c>
+      <c r="N39" s="4" t="n">
+        <f aca="false">STDEV(N2:N36)</f>
+        <v>0.0391040471894796</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="3" t="n">
+      <c r="B40" s="4" t="n">
         <f aca="false">MEDIAN(B2:B36)</f>
         <v>0</v>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="4" t="n">
         <f aca="false">MEDIAN(C2:C36)</f>
         <v>0</v>
       </c>
-      <c r="D40" s="3" t="n">
+      <c r="D40" s="4" t="n">
         <f aca="false">MEDIAN(D2:D36)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="3" t="n">
+      <c r="E40" s="4" t="n">
         <f aca="false">MEDIAN(E2:E36)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="3" t="n">
+      <c r="F40" s="4" t="n">
         <f aca="false">MEDIAN(F2:F36)</f>
         <v>0</v>
       </c>
-      <c r="G40" s="3" t="n">
+      <c r="G40" s="4" t="n">
         <f aca="false">MEDIAN(G2:G36)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="4" t="n">
+        <f aca="false">MEDIAN(I2:I36)</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="4" t="n">
+        <f aca="false">MEDIAN(J2:J36)</f>
+        <v>0</v>
+      </c>
+      <c r="K40" s="4" t="n">
+        <f aca="false">MEDIAN(K2:K36)</f>
+        <v>0</v>
+      </c>
+      <c r="L40" s="4" t="n">
+        <f aca="false">MEDIAN(L2:L36)</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="4" t="n">
+        <f aca="false">MEDIAN(M2:M36)</f>
+        <v>4.16333634234434E-017</v>
+      </c>
+      <c r="N40" s="4" t="n">
+        <f aca="false">MEDIAN(N2:N36)</f>
         <v>0</v>
       </c>
     </row>
@@ -2140,58 +2098,106 @@
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="3" t="n">
+      <c r="B41" s="4" t="n">
         <f aca="false">MIN(B2:B36)</f>
         <v>-0.154781060861362</v>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="4" t="n">
         <f aca="false">MIN(C2:C36)</f>
         <v>-0.167328162431212</v>
       </c>
-      <c r="D41" s="3" t="n">
+      <c r="D41" s="4" t="n">
         <f aca="false">MIN(D2:D36)</f>
         <v>-0.163737569060625</v>
       </c>
-      <c r="E41" s="3" t="n">
+      <c r="E41" s="4" t="n">
         <f aca="false">MIN(E2:E36)</f>
         <v>-0.167328162431212</v>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="F41" s="4" t="n">
         <f aca="false">MIN(F2:F36)</f>
         <v>-0.184986266311087</v>
       </c>
-      <c r="G41" s="3" t="n">
+      <c r="G41" s="4" t="n">
         <f aca="false">MIN(G2:G36)</f>
         <v>-0.1682060420022</v>
+      </c>
+      <c r="I41" s="4" t="n">
+        <f aca="false">MIN(I2:I36)</f>
+        <v>-0.133597647995575</v>
+      </c>
+      <c r="J41" s="4" t="n">
+        <f aca="false">MIN(J2:J36)</f>
+        <v>-0.167328162431212</v>
+      </c>
+      <c r="K41" s="4" t="n">
+        <f aca="false">MIN(K2:K36)</f>
+        <v>-0.163737569060625</v>
+      </c>
+      <c r="L41" s="4" t="n">
+        <f aca="false">MIN(L2:L36)</f>
+        <v>-0.167328162431212</v>
+      </c>
+      <c r="M41" s="4" t="n">
+        <f aca="false">MIN(M2:M36)</f>
+        <v>-0.148531108575075</v>
+      </c>
+      <c r="N41" s="4" t="n">
+        <f aca="false">MIN(N2:N36)</f>
+        <v>-0.164606116063325</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="3" t="n">
+      <c r="B42" s="4" t="n">
         <f aca="false">MAX(B2:B36)</f>
         <v>0.2778478008989</v>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" s="4" t="n">
         <f aca="false">MAX(C2:C36)</f>
         <v>0.29054158741485</v>
       </c>
-      <c r="D42" s="3" t="n">
+      <c r="D42" s="4" t="n">
         <f aca="false">MAX(D2:D36)</f>
         <v>0.193677566673</v>
       </c>
-      <c r="E42" s="3" t="n">
+      <c r="E42" s="4" t="n">
         <f aca="false">MAX(E2:E36)</f>
         <v>0.2620481196488</v>
       </c>
-      <c r="F42" s="3" t="n">
+      <c r="F42" s="4" t="n">
         <f aca="false">MAX(F2:F36)</f>
         <v>0.0782993526029253</v>
       </c>
-      <c r="G42" s="3" t="n">
+      <c r="G42" s="4" t="n">
         <f aca="false">MAX(G2:G36)</f>
         <v>0.0462446815015131</v>
+      </c>
+      <c r="I42" s="4" t="n">
+        <f aca="false">MAX(I2:I36)</f>
+        <v>0.2778478008989</v>
+      </c>
+      <c r="J42" s="4" t="n">
+        <f aca="false">MAX(J2:J36)</f>
+        <v>0.144502246056187</v>
+      </c>
+      <c r="K42" s="4" t="n">
+        <f aca="false">MAX(K2:K36)</f>
+        <v>0.193677566673</v>
+      </c>
+      <c r="L42" s="4" t="n">
+        <f aca="false">MAX(L2:L36)</f>
+        <v>0.116008778290138</v>
+      </c>
+      <c r="M42" s="4" t="n">
+        <f aca="false">MAX(M2:M36)</f>
+        <v>0.0480260896533753</v>
+      </c>
+      <c r="N42" s="4" t="n">
+        <f aca="false">MAX(N2:N36)</f>
+        <v>0.0443855028395253</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2222,6 +2228,30 @@
         <f aca="false">COUNTIF(G2:G36,"&gt;=0")</f>
         <v>19</v>
       </c>
+      <c r="I43" s="0" t="n">
+        <f aca="false">COUNTIF(I2:I36,"&gt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <f aca="false">COUNTIF(J2:J36,"&gt;=0")</f>
+        <v>20</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <f aca="false">COUNTIF(K2:K36,"&gt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <f aca="false">COUNTIF(L2:L36,"&gt;=0")</f>
+        <v>20</v>
+      </c>
+      <c r="M43" s="0" t="n">
+        <f aca="false">COUNTIF(M2:M36,"&gt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="N43" s="0" t="n">
+        <f aca="false">COUNTIF(N2:N36,"&gt;=0")</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
@@ -2250,6 +2280,30 @@
       <c r="G44" s="0" t="n">
         <f aca="false">COUNTIF(G2:G36,"&lt;0")</f>
         <v>16</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <f aca="false">COUNTIF(I2:I36,"&lt;0")</f>
+        <v>16</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <f aca="false">COUNTIF(J2:J36,"&lt;0")</f>
+        <v>15</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <f aca="false">COUNTIF(K2:K36,"&lt;0")</f>
+        <v>16</v>
+      </c>
+      <c r="L44" s="0" t="n">
+        <f aca="false">COUNTIF(L2:L36,"&lt;0")</f>
+        <v>15</v>
+      </c>
+      <c r="M44" s="0" t="n">
+        <f aca="false">COUNTIF(M2:M36,"&lt;0")</f>
+        <v>16</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <f aca="false">COUNTIF(N2:N36,"&lt;0")</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2276,11 +2330,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7142857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2325,10 +2377,10 @@
       <c r="D2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G2" s="0" t="s">
@@ -2337,7 +2389,7 @@
       <c r="H2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="4" t="n">
         <f aca="false">HLOOKUP(A2,AQ_results!$A$1:$G$44,38,0)</f>
         <v>-0.00479083054900702</v>
       </c>
@@ -2355,10 +2407,10 @@
       <c r="D3" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -2367,7 +2419,7 @@
       <c r="H3" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="4" t="n">
         <f aca="false">HLOOKUP(A3,AQ_results!$A$1:$G$44,38,0)</f>
         <v>0.00322423676433478</v>
       </c>
@@ -2385,10 +2437,10 @@
       <c r="D4" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G4" s="0" t="s">
@@ -2397,7 +2449,7 @@
       <c r="H4" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="4" t="n">
         <f aca="false">HLOOKUP(A4,AQ_results!$A$1:$G$44,38,0)</f>
         <v>-0.0107325392898438</v>
       </c>
@@ -2415,10 +2467,10 @@
       <c r="D5" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -2427,7 +2479,7 @@
       <c r="H5" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="4" t="n">
         <f aca="false">HLOOKUP(A5,AQ_results!$A$1:$G$44,38,0)</f>
         <v>-0.00217132647935524</v>
       </c>
@@ -2445,10 +2497,10 @@
       <c r="D6" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G6" s="0" t="s">
@@ -2457,7 +2509,7 @@
       <c r="H6" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="4" t="n">
         <f aca="false">HLOOKUP(A6,AQ_results!$A$1:$G$44,38,0)</f>
         <v>-0.0127465419698248</v>
       </c>
@@ -2475,10 +2527,10 @@
       <c r="D7" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G7" s="0" t="s">
@@ -2487,7 +2539,7 @@
       <c r="H7" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="4" t="n">
         <f aca="false">HLOOKUP(A7,AQ_results!$A$1:$G$44,38,0)</f>
         <v>-0.00983365728067769</v>
       </c>
@@ -2511,16 +2563,14 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="2" style="0" width="13.9336734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.7704081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="20.1938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="2" style="0" width="14.1479591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="20.8418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,22 +2596,22 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2639,7 +2689,7 @@
       </c>
       <c r="J3" s="2" t="n">
         <f aca="false">J2+C3</f>
-        <v>-0.0458916924579366</v>
+        <v>-0.0458916924579365</v>
       </c>
       <c r="K3" s="2" t="n">
         <f aca="false">K2+D3</f>
@@ -2647,7 +2697,7 @@
       </c>
       <c r="L3" s="2" t="n">
         <f aca="false">L2+E3</f>
-        <v>-0.0577407667593362</v>
+        <v>-0.0577407667593361</v>
       </c>
       <c r="M3" s="2" t="n">
         <f aca="false">M2+F3</f>
@@ -2655,7 +2705,7 @@
       </c>
       <c r="N3" s="2" t="n">
         <f aca="false">N2+G3</f>
-        <v>-0.0728770194710984</v>
+        <v>-0.0728770194710983</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2680,18 +2730,18 @@
       <c r="G4" s="2" t="n">
         <v>0.0176142794282254</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="4"/>
       <c r="I4" s="2" t="n">
         <f aca="false">I3+B4</f>
         <v>-0.180742327160961</v>
       </c>
       <c r="J4" s="2" t="n">
         <f aca="false">J3+C4</f>
-        <v>-0.0266880403809364</v>
+        <v>-0.0266880403809363</v>
       </c>
       <c r="K4" s="2" t="n">
         <f aca="false">K3+D4</f>
-        <v>-0.185900385439236</v>
+        <v>-0.185900385439235</v>
       </c>
       <c r="L4" s="2" t="n">
         <f aca="false">L3+E4</f>
@@ -2703,7 +2753,7 @@
       </c>
       <c r="N4" s="2" t="n">
         <f aca="false">N3+G4</f>
-        <v>-0.055262740042873</v>
+        <v>-0.0552627400428729</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2734,11 +2784,11 @@
       </c>
       <c r="J5" s="2" t="n">
         <f aca="false">J4+C5</f>
-        <v>0.0796765712101513</v>
+        <v>0.0796765712101517</v>
       </c>
       <c r="K5" s="2" t="n">
         <f aca="false">K4+D5</f>
-        <v>-0.116030668086448</v>
+        <v>-0.116030668086447</v>
       </c>
       <c r="L5" s="2" t="n">
         <f aca="false">L4+E5</f>
@@ -2777,15 +2827,15 @@
       </c>
       <c r="I6" s="2" t="n">
         <f aca="false">I5+B6</f>
-        <v>0.0290850778107398</v>
+        <v>0.0290850778107396</v>
       </c>
       <c r="J6" s="2" t="n">
         <f aca="false">J5+C6</f>
-        <v>0.0484470504870019</v>
+        <v>0.0484470504870024</v>
       </c>
       <c r="K6" s="2" t="n">
         <f aca="false">K5+D6</f>
-        <v>-0.0594821910670971</v>
+        <v>-0.0594821910670967</v>
       </c>
       <c r="L6" s="2" t="n">
         <f aca="false">L5+E6</f>
@@ -2824,7 +2874,7 @@
       </c>
       <c r="I7" s="2" t="n">
         <f aca="false">I6+B7</f>
-        <v>-0.097509926045448</v>
+        <v>-0.0975099260454484</v>
       </c>
       <c r="J7" s="2" t="n">
         <f aca="false">J6+C7</f>
@@ -2832,7 +2882,7 @@
       </c>
       <c r="K7" s="2" t="n">
         <f aca="false">K6+D7</f>
-        <v>-0.0669457940382844</v>
+        <v>-0.066945794038284</v>
       </c>
       <c r="L7" s="2" t="n">
         <f aca="false">L6+E7</f>
@@ -2875,7 +2925,7 @@
       </c>
       <c r="J8" s="2" t="n">
         <f aca="false">J7+C8</f>
-        <v>0.0213673518088407</v>
+        <v>0.0213673518088411</v>
       </c>
       <c r="K8" s="2" t="n">
         <f aca="false">K7+D8</f>
@@ -2883,15 +2933,15 @@
       </c>
       <c r="L8" s="2" t="n">
         <f aca="false">L7+E8</f>
-        <v>0.000751589302241174</v>
+        <v>0.000751589302241049</v>
       </c>
       <c r="M8" s="2" t="n">
         <f aca="false">M7+F8</f>
-        <v>-0.240775171960546</v>
+        <v>-0.240775171960547</v>
       </c>
       <c r="N8" s="2" t="n">
         <f aca="false">N7+G8</f>
-        <v>-0.089024059001146</v>
+        <v>-0.0890240590011459</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2922,7 +2972,7 @@
       </c>
       <c r="J9" s="2" t="n">
         <f aca="false">J8+C9</f>
-        <v>0.0285206110486031</v>
+        <v>0.0285206110486036</v>
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">K8+D9</f>
@@ -2930,15 +2980,15 @@
       </c>
       <c r="L9" s="2" t="n">
         <f aca="false">L8+E9</f>
-        <v>0.00821845029604115</v>
+        <v>0.00821845029604103</v>
       </c>
       <c r="M9" s="2" t="n">
         <f aca="false">M8+F9</f>
-        <v>-0.239855355546871</v>
+        <v>-0.239855355546872</v>
       </c>
       <c r="N9" s="2" t="n">
         <f aca="false">N8+G9</f>
-        <v>-0.101029944446671</v>
+        <v>-0.10102994444667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2969,7 +3019,7 @@
       </c>
       <c r="J10" s="2" t="n">
         <f aca="false">J9+C10</f>
-        <v>-0.0156773011058966</v>
+        <v>-0.0156773011058962</v>
       </c>
       <c r="K10" s="2" t="n">
         <f aca="false">K9+D10</f>
@@ -2977,15 +3027,15 @@
       </c>
       <c r="L10" s="2" t="n">
         <f aca="false">L9+E10</f>
-        <v>-0.0407586947711089</v>
+        <v>-0.040758694771109</v>
       </c>
       <c r="M10" s="2" t="n">
         <f aca="false">M9+F10</f>
-        <v>-0.239855355546871</v>
+        <v>-0.239855355546872</v>
       </c>
       <c r="N10" s="2" t="n">
         <f aca="false">N9+G10</f>
-        <v>-0.101029944446671</v>
+        <v>-0.10102994444667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3016,7 +3066,7 @@
       </c>
       <c r="J11" s="2" t="n">
         <f aca="false">J10+C11</f>
-        <v>-0.0537327907293335</v>
+        <v>-0.0537327907293331</v>
       </c>
       <c r="K11" s="2" t="n">
         <f aca="false">K10+D11</f>
@@ -3024,7 +3074,7 @@
       </c>
       <c r="L11" s="2" t="n">
         <f aca="false">L10+E11</f>
-        <v>-0.0788141843945458</v>
+        <v>-0.0788141843945459</v>
       </c>
       <c r="M11" s="2" t="n">
         <f aca="false">M10+F11</f>
@@ -3063,7 +3113,7 @@
       </c>
       <c r="J12" s="2" t="n">
         <f aca="false">J11+C12</f>
-        <v>-0.0382428789004333</v>
+        <v>-0.0382428789004328</v>
       </c>
       <c r="K12" s="2" t="n">
         <f aca="false">K11+D12</f>
@@ -3071,11 +3121,11 @@
       </c>
       <c r="L12" s="2" t="n">
         <f aca="false">L11+E12</f>
-        <v>-0.0633242725656455</v>
+        <v>-0.0633242725656456</v>
       </c>
       <c r="M12" s="2" t="n">
         <f aca="false">M11+F12</f>
-        <v>-0.297026401097308</v>
+        <v>-0.297026401097309</v>
       </c>
       <c r="N12" s="2" t="n">
         <f aca="false">N11+G12</f>
@@ -3110,7 +3160,7 @@
       </c>
       <c r="J13" s="2" t="n">
         <f aca="false">J12+C13</f>
-        <v>-0.0791712744608083</v>
+        <v>-0.0791712744608078</v>
       </c>
       <c r="K13" s="2" t="n">
         <f aca="false">K12+D13</f>
@@ -3153,15 +3203,15 @@
       </c>
       <c r="I14" s="2" t="n">
         <f aca="false">I13+B14</f>
-        <v>-0.336166209469209</v>
+        <v>-0.33616620946921</v>
       </c>
       <c r="J14" s="2" t="n">
         <f aca="false">J13+C14</f>
-        <v>-0.0297813822433701</v>
+        <v>-0.0297813822433697</v>
       </c>
       <c r="K14" s="2" t="n">
         <f aca="false">K13+D14</f>
-        <v>-0.300940520480859</v>
+        <v>-0.300940520480858</v>
       </c>
       <c r="L14" s="2" t="n">
         <f aca="false">L13+E14</f>
@@ -3200,15 +3250,15 @@
       </c>
       <c r="I15" s="2" t="n">
         <f aca="false">I14+B15</f>
-        <v>-0.307678723341434</v>
+        <v>-0.307678723341435</v>
       </c>
       <c r="J15" s="2" t="n">
         <f aca="false">J14+C15</f>
-        <v>-0.0115685175047952</v>
+        <v>-0.0115685175047949</v>
       </c>
       <c r="K15" s="2" t="n">
         <f aca="false">K14+D15</f>
-        <v>-0.289286724286959</v>
+        <v>-0.289286724286958</v>
       </c>
       <c r="L15" s="2" t="n">
         <f aca="false">L14+E15</f>
@@ -3251,7 +3301,7 @@
       </c>
       <c r="J16" s="2" t="n">
         <f aca="false">J15+C16</f>
-        <v>-0.0278891538279199</v>
+        <v>-0.0278891538279196</v>
       </c>
       <c r="K16" s="2" t="n">
         <f aca="false">K15+D16</f>
@@ -3298,7 +3348,7 @@
       </c>
       <c r="J17" s="2" t="n">
         <f aca="false">J16+C17</f>
-        <v>-0.0139685167086199</v>
+        <v>-0.0139685167086196</v>
       </c>
       <c r="K17" s="2" t="n">
         <f aca="false">K16+D17</f>
@@ -3306,7 +3356,7 @@
       </c>
       <c r="L17" s="2" t="n">
         <f aca="false">L16+E17</f>
-        <v>-0.0742714248618951</v>
+        <v>-0.0742714248618952</v>
       </c>
       <c r="M17" s="2" t="n">
         <f aca="false">M16+F17</f>
@@ -3345,7 +3395,7 @@
       </c>
       <c r="J18" s="2" t="n">
         <f aca="false">J17+C18</f>
-        <v>0.00552953006623016</v>
+        <v>0.00552953006623055</v>
       </c>
       <c r="K18" s="2" t="n">
         <f aca="false">K17+D18</f>
@@ -3392,7 +3442,7 @@
       </c>
       <c r="J19" s="2" t="n">
         <f aca="false">J18+C19</f>
-        <v>0.0292539965726053</v>
+        <v>0.0292539965726056</v>
       </c>
       <c r="K19" s="2" t="n">
         <f aca="false">K18+D19</f>
@@ -3400,7 +3450,7 @@
       </c>
       <c r="L19" s="2" t="n">
         <f aca="false">L18+E19</f>
-        <v>0.0758100818688548</v>
+        <v>0.0758100818688549</v>
       </c>
       <c r="M19" s="2" t="n">
         <f aca="false">M18+F19</f>
@@ -3439,7 +3489,7 @@
       </c>
       <c r="J20" s="2" t="n">
         <f aca="false">J19+C20</f>
-        <v>-0.0428282519700697</v>
+        <v>-0.0428282519700694</v>
       </c>
       <c r="K20" s="2" t="n">
         <f aca="false">K19+D20</f>
@@ -3447,7 +3497,7 @@
       </c>
       <c r="L20" s="2" t="n">
         <f aca="false">L19+E20</f>
-        <v>0.0936316455357298</v>
+        <v>0.0936316455357299</v>
       </c>
       <c r="M20" s="2" t="n">
         <f aca="false">M19+F20</f>
@@ -3482,15 +3532,15 @@
       </c>
       <c r="I21" s="2" t="n">
         <f aca="false">I20+B21</f>
-        <v>-0.315528180953808</v>
+        <v>-0.315528180953809</v>
       </c>
       <c r="J21" s="2" t="n">
         <f aca="false">J20+C21</f>
-        <v>-0.0743358531569947</v>
+        <v>-0.0743358531569944</v>
       </c>
       <c r="K21" s="2" t="n">
         <f aca="false">K20+D21</f>
-        <v>-0.262107561671958</v>
+        <v>-0.262107561671957</v>
       </c>
       <c r="L21" s="2" t="n">
         <f aca="false">L20+E21</f>
@@ -3529,15 +3579,15 @@
       </c>
       <c r="I22" s="2" t="n">
         <f aca="false">I21+B22</f>
-        <v>-0.300615287589433</v>
+        <v>-0.300615287589434</v>
       </c>
       <c r="J22" s="2" t="n">
         <f aca="false">J21+C22</f>
-        <v>-0.0594785143849695</v>
+        <v>-0.0594785143849692</v>
       </c>
       <c r="K22" s="2" t="n">
         <f aca="false">K21+D22</f>
-        <v>-0.247194668307583</v>
+        <v>-0.247194668307582</v>
       </c>
       <c r="L22" s="2" t="n">
         <f aca="false">L21+E22</f>
@@ -3580,7 +3630,7 @@
       </c>
       <c r="J23" s="2" t="n">
         <f aca="false">J22+C23</f>
-        <v>-0.071974290166244</v>
+        <v>-0.0719742901662437</v>
       </c>
       <c r="K23" s="2" t="n">
         <f aca="false">K22+D23</f>
@@ -3627,7 +3677,7 @@
       </c>
       <c r="J24" s="2" t="n">
         <f aca="false">J23+C24</f>
-        <v>-0.071974290166244</v>
+        <v>-0.0719742901662437</v>
       </c>
       <c r="K24" s="2" t="n">
         <f aca="false">K23+D24</f>
@@ -3674,7 +3724,7 @@
       </c>
       <c r="J25" s="2" t="n">
         <f aca="false">J24+C25</f>
-        <v>-0.0416145105839188</v>
+        <v>-0.0416145105839185</v>
       </c>
       <c r="K25" s="2" t="n">
         <f aca="false">K24+D25</f>
@@ -3682,7 +3732,7 @@
       </c>
       <c r="L25" s="2" t="n">
         <f aca="false">L24+E25</f>
-        <v>-0.00286240557114389</v>
+        <v>-0.00286240557114385</v>
       </c>
       <c r="M25" s="2" t="n">
         <f aca="false">M24+F25</f>
@@ -3721,7 +3771,7 @@
       </c>
       <c r="J26" s="2" t="n">
         <f aca="false">J25+C26</f>
-        <v>-0.0750764640995686</v>
+        <v>-0.0750764640995683</v>
       </c>
       <c r="K26" s="2" t="n">
         <f aca="false">K25+D26</f>
@@ -3764,23 +3814,23 @@
       </c>
       <c r="I27" s="2" t="n">
         <f aca="false">I26+B27</f>
-        <v>-0.382580190749582</v>
+        <v>-0.382580190749583</v>
       </c>
       <c r="J27" s="2" t="n">
         <f aca="false">J26+C27</f>
-        <v>-0.0807868533424186</v>
+        <v>-0.0807868533424182</v>
       </c>
       <c r="K27" s="2" t="n">
         <f aca="false">K26+D27</f>
-        <v>-0.277994447794907</v>
+        <v>-0.277994447794906</v>
       </c>
       <c r="L27" s="2" t="n">
         <f aca="false">L26+E27</f>
-        <v>-0.0357993548901187</v>
+        <v>-0.0357993548901186</v>
       </c>
       <c r="M27" s="2" t="n">
         <f aca="false">M26+F27</f>
-        <v>-0.442391227184456</v>
+        <v>-0.442391227184457</v>
       </c>
       <c r="N27" s="2" t="n">
         <f aca="false">N26+G27</f>
@@ -3811,23 +3861,23 @@
       </c>
       <c r="I28" s="2" t="n">
         <f aca="false">I27+B28</f>
-        <v>-0.382580190749582</v>
+        <v>-0.382580190749583</v>
       </c>
       <c r="J28" s="2" t="n">
         <f aca="false">J27+C28</f>
-        <v>-0.0807868533424186</v>
+        <v>-0.0807868533424182</v>
       </c>
       <c r="K28" s="2" t="n">
         <f aca="false">K27+D28</f>
-        <v>-0.277994447794907</v>
+        <v>-0.277994447794906</v>
       </c>
       <c r="L28" s="2" t="n">
         <f aca="false">L27+E28</f>
-        <v>-0.0357993548901187</v>
+        <v>-0.0357993548901186</v>
       </c>
       <c r="M28" s="2" t="n">
         <f aca="false">M27+F28</f>
-        <v>-0.442391227184456</v>
+        <v>-0.442391227184457</v>
       </c>
       <c r="N28" s="2" t="n">
         <f aca="false">N27+G28</f>
@@ -3862,15 +3912,15 @@
       </c>
       <c r="J29" s="2" t="n">
         <f aca="false">J28+C29</f>
-        <v>-0.0805189461108683</v>
+        <v>-0.0805189461108679</v>
       </c>
       <c r="K29" s="2" t="n">
         <f aca="false">K28+D29</f>
-        <v>-0.285691356583982</v>
+        <v>-0.285691356583981</v>
       </c>
       <c r="L29" s="2" t="n">
         <f aca="false">L28+E29</f>
-        <v>-0.0575272222779437</v>
+        <v>-0.0575272222779436</v>
       </c>
       <c r="M29" s="2" t="n">
         <f aca="false">M28+F29</f>
@@ -3909,7 +3959,7 @@
       </c>
       <c r="J30" s="2" t="n">
         <f aca="false">J29+C30</f>
-        <v>-0.0789405971825932</v>
+        <v>-0.0789405971825928</v>
       </c>
       <c r="K30" s="2" t="n">
         <f aca="false">K29+D30</f>
@@ -3917,7 +3967,7 @@
       </c>
       <c r="L30" s="2" t="n">
         <f aca="false">L29+E30</f>
-        <v>-0.0559488733496686</v>
+        <v>-0.0559488733496685</v>
       </c>
       <c r="M30" s="2" t="n">
         <f aca="false">M29+F30</f>
@@ -3956,7 +4006,7 @@
       </c>
       <c r="J31" s="2" t="n">
         <f aca="false">J30+C31</f>
-        <v>-0.0635520136939931</v>
+        <v>-0.0635520136939927</v>
       </c>
       <c r="K31" s="2" t="n">
         <f aca="false">K30+D31</f>
@@ -3964,7 +4014,7 @@
       </c>
       <c r="L31" s="2" t="n">
         <f aca="false">L30+E31</f>
-        <v>-0.0405602898610685</v>
+        <v>-0.0405602898610684</v>
       </c>
       <c r="M31" s="2" t="n">
         <f aca="false">M30+F31</f>
@@ -4003,7 +4053,7 @@
       </c>
       <c r="J32" s="2" t="n">
         <f aca="false">J31+C32</f>
-        <v>-0.0754062535427433</v>
+        <v>-0.0754062535427429</v>
       </c>
       <c r="K32" s="2" t="n">
         <f aca="false">K31+D32</f>
@@ -4011,7 +4061,7 @@
       </c>
       <c r="L32" s="2" t="n">
         <f aca="false">L31+E32</f>
-        <v>-0.0368889287332686</v>
+        <v>-0.0368889287332685</v>
       </c>
       <c r="M32" s="2" t="n">
         <f aca="false">M31+F32</f>
@@ -4050,7 +4100,7 @@
       </c>
       <c r="J33" s="2" t="n">
         <f aca="false">J32+C33</f>
-        <v>-0.050373302756493</v>
+        <v>-0.0503733027564926</v>
       </c>
       <c r="K33" s="2" t="n">
         <f aca="false">K32+D33</f>
@@ -4058,11 +4108,11 @@
       </c>
       <c r="L33" s="2" t="n">
         <f aca="false">L32+E33</f>
-        <v>-0.0118559779470183</v>
+        <v>-0.0118559779470182</v>
       </c>
       <c r="M33" s="2" t="n">
         <f aca="false">M32+F33</f>
-        <v>-0.30683845842948</v>
+        <v>-0.306838458429481</v>
       </c>
       <c r="N33" s="2" t="n">
         <f aca="false">N32+G33</f>
@@ -4093,11 +4143,11 @@
       </c>
       <c r="I34" s="2" t="n">
         <f aca="false">I33+B34</f>
-        <v>-0.382690680578381</v>
+        <v>-0.382690680578382</v>
       </c>
       <c r="J34" s="2" t="n">
         <f aca="false">J33+C34</f>
-        <v>-0.046842393581793</v>
+        <v>-0.0468423935817925</v>
       </c>
       <c r="K34" s="2" t="n">
         <f aca="false">K33+D34</f>
@@ -4105,7 +4155,7 @@
       </c>
       <c r="L34" s="2" t="n">
         <f aca="false">L33+E34</f>
-        <v>-0.0361667435770186</v>
+        <v>-0.0361667435770185</v>
       </c>
       <c r="M34" s="2" t="n">
         <f aca="false">M33+F34</f>
@@ -4140,11 +4190,11 @@
       </c>
       <c r="I35" s="2" t="n">
         <f aca="false">I34+B35</f>
-        <v>-0.475046143368856</v>
+        <v>-0.475046143368857</v>
       </c>
       <c r="J35" s="2" t="n">
         <f aca="false">J34+C35</f>
-        <v>-0.129573893882268</v>
+        <v>-0.129573893882267</v>
       </c>
       <c r="K35" s="2" t="n">
         <f aca="false">K34+D35</f>
@@ -4195,7 +4245,7 @@
       </c>
       <c r="K36" s="2" t="n">
         <f aca="false">K35+D36</f>
-        <v>-0.244550751025206</v>
+        <v>-0.244550751025205</v>
       </c>
       <c r="L36" s="2" t="n">
         <f aca="false">L35+E36</f>
@@ -4214,27 +4264,27 @@
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="3" t="n">
+      <c r="B38" s="4" t="n">
         <f aca="false">AVERAGE(B2:B36)</f>
         <v>-0.0148394403293702</v>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="4" t="n">
         <f aca="false">AVERAGE(C2:C36)</f>
-        <v>-0.00479706528236979</v>
-      </c>
-      <c r="D38" s="3" t="n">
+        <v>-0.00479706528236977</v>
+      </c>
+      <c r="D38" s="4" t="n">
         <f aca="false">AVERAGE(D2:D36)</f>
         <v>-0.00698716431500588</v>
       </c>
-      <c r="E38" s="3" t="n">
+      <c r="E38" s="4" t="n">
         <f aca="false">AVERAGE(E2:E36)</f>
-        <v>-0.00448544095187624</v>
-      </c>
-      <c r="F38" s="3" t="n">
+        <v>-0.00448544095187623</v>
+      </c>
+      <c r="F38" s="4" t="n">
         <f aca="false">AVERAGE(F2:F36)</f>
         <v>-0.0121176996131244</v>
       </c>
-      <c r="G38" s="3" t="n">
+      <c r="G38" s="4" t="n">
         <f aca="false">AVERAGE(G2:G36)</f>
         <v>-0.00976170532404834</v>
       </c>
@@ -4243,27 +4293,27 @@
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="3" t="n">
+      <c r="B39" s="4" t="n">
         <f aca="false">STDEV(B2:B36)</f>
         <v>0.0579070346502453</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="4" t="n">
         <f aca="false">STDEV(C2:C36)</f>
         <v>0.040193227832285</v>
       </c>
-      <c r="D39" s="3" t="n">
+      <c r="D39" s="4" t="n">
         <f aca="false">STDEV(D2:D36)</f>
         <v>0.0477249124399749</v>
       </c>
-      <c r="E39" s="3" t="n">
+      <c r="E39" s="4" t="n">
         <f aca="false">STDEV(E2:E36)</f>
         <v>0.0591006548613329</v>
       </c>
-      <c r="F39" s="3" t="n">
+      <c r="F39" s="4" t="n">
         <f aca="false">STDEV(F2:F36)</f>
         <v>0.0454715868078014</v>
       </c>
-      <c r="G39" s="3" t="n">
+      <c r="G39" s="4" t="n">
         <f aca="false">STDEV(G2:G36)</f>
         <v>0.0460960512437212</v>
       </c>
@@ -4272,27 +4322,27 @@
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="3" t="n">
+      <c r="B40" s="4" t="n">
         <f aca="false">MEDIAN(B2:B36)</f>
         <v>0</v>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="4" t="n">
         <f aca="false">MEDIAN(C2:C36)</f>
         <v>0.00026790723155027</v>
       </c>
-      <c r="D40" s="3" t="n">
+      <c r="D40" s="4" t="n">
         <f aca="false">MEDIAN(D2:D36)</f>
         <v>0.00157834892827511</v>
       </c>
-      <c r="E40" s="3" t="n">
+      <c r="E40" s="4" t="n">
         <f aca="false">MEDIAN(E2:E36)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="3" t="n">
+      <c r="F40" s="4" t="n">
         <f aca="false">MEDIAN(F2:F36)</f>
         <v>0</v>
       </c>
-      <c r="G40" s="3" t="n">
+      <c r="G40" s="4" t="n">
         <f aca="false">MEDIAN(G2:G36)</f>
         <v>0</v>
       </c>
@@ -4301,27 +4351,27 @@
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="3" t="n">
+      <c r="B41" s="4" t="n">
         <f aca="false">MIN(B2:B36)</f>
         <v>-0.160197218683762</v>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="4" t="n">
         <f aca="false">MIN(C2:C36)</f>
         <v>-0.0827315003004748</v>
       </c>
-      <c r="D41" s="3" t="n">
+      <c r="D41" s="4" t="n">
         <f aca="false">MIN(D2:D36)</f>
         <v>-0.160907838042186</v>
       </c>
-      <c r="E41" s="3" t="n">
+      <c r="E41" s="4" t="n">
         <f aca="false">MIN(E2:E36)</f>
         <v>-0.109927098948412</v>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="F41" s="4" t="n">
         <f aca="false">MIN(F2:F36)</f>
         <v>-0.120569765226862</v>
       </c>
-      <c r="G41" s="3" t="n">
+      <c r="G41" s="4" t="n">
         <f aca="false">MIN(G2:G36)</f>
         <v>-0.113160874141174</v>
       </c>
@@ -4330,27 +4380,27 @@
       <c r="A42" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="3" t="n">
+      <c r="B42" s="4" t="n">
         <f aca="false">MAX(B2:B36)</f>
         <v>0.139957687618913</v>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" s="4" t="n">
         <f aca="false">MAX(C2:C36)</f>
         <v>0.106364611591088</v>
       </c>
-      <c r="D42" s="3" t="n">
+      <c r="D42" s="4" t="n">
         <f aca="false">MAX(D2:D36)</f>
         <v>0.0698697173527877</v>
       </c>
-      <c r="E42" s="3" t="n">
+      <c r="E42" s="4" t="n">
         <f aca="false">MAX(E2:E36)</f>
         <v>0.20971038582105</v>
       </c>
-      <c r="F42" s="3" t="n">
+      <c r="F42" s="4" t="n">
         <f aca="false">MAX(F2:F36)</f>
         <v>0.0967803177834504</v>
       </c>
-      <c r="G42" s="3" t="n">
+      <c r="G42" s="4" t="n">
         <f aca="false">MAX(G2:G36)</f>
         <v>0.0896686446188374</v>
       </c>
@@ -4431,17 +4481,15 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7142857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4486,10 +4534,10 @@
       <c r="D2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G2" s="0" t="s">
@@ -4498,7 +4546,7 @@
       <c r="H2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="4" t="n">
         <f aca="false">HLOOKUP(A2,CN2_results!$A$1:$G$44,38,0)</f>
         <v>-0.0148394403293702</v>
       </c>
@@ -4516,10 +4564,10 @@
       <c r="D3" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -4528,9 +4576,9 @@
       <c r="H3" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="4" t="n">
         <f aca="false">HLOOKUP(A3,CN2_results!$A$1:$G$44,38,0)</f>
-        <v>-0.00479706528236979</v>
+        <v>-0.00479706528236977</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4546,10 +4594,10 @@
       <c r="D4" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G4" s="0" t="s">
@@ -4558,7 +4606,7 @@
       <c r="H4" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="4" t="n">
         <f aca="false">HLOOKUP(A4,CN2_results!$A$1:$G$44,38,0)</f>
         <v>-0.00698716431500588</v>
       </c>
@@ -4576,10 +4624,10 @@
       <c r="D5" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -4588,9 +4636,9 @@
       <c r="H5" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="4" t="n">
         <f aca="false">HLOOKUP(A5,CN2_results!$A$1:$G$44,38,0)</f>
-        <v>-0.00448544095187624</v>
+        <v>-0.00448544095187623</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4606,10 +4654,10 @@
       <c r="D6" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G6" s="0" t="s">
@@ -4618,7 +4666,7 @@
       <c r="H6" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="4" t="n">
         <f aca="false">HLOOKUP(A6,CN2_results!$A$1:$G$44,38,0)</f>
         <v>-0.0121176996131244</v>
       </c>
@@ -4636,10 +4684,10 @@
       <c r="D7" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="G7" s="0" t="s">
@@ -4648,9 +4696,100 @@
       <c r="H7" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="4" t="n">
         <f aca="false">HLOOKUP(A7,CN2_results!$A$1:$G$44,38,0)</f>
         <v>-0.00976170532404834</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.6632653061225"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>